<commit_message>
Updated games  table a bit
</commit_message>
<xml_diff>
--- a/GameDB.xlsx
+++ b/GameDB.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6F8ABF7C-3E25-498C-9418-8D32170F1E2D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50B1462F-0A43-4BD0-8CF1-9C046F165D18}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Game" sheetId="2" r:id="rId1"/>
@@ -16,17 +16,22 @@
     <sheet name="Manufacturer" sheetId="4" r:id="rId6"/>
     <sheet name="ESRB" sheetId="6" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="62">
   <si>
     <t>Name</t>
   </si>
@@ -149,6 +154,69 @@
   </si>
   <si>
     <t>Xbox</t>
+  </si>
+  <si>
+    <t>Missile Command</t>
+  </si>
+  <si>
+    <t>Crash Bandicoot</t>
+  </si>
+  <si>
+    <t>Star Wars Battlefront</t>
+  </si>
+  <si>
+    <t>Halo Reach</t>
+  </si>
+  <si>
+    <t>Guitar Hero: On Tour</t>
+  </si>
+  <si>
+    <t>Monster Hunter World</t>
+  </si>
+  <si>
+    <t>Mario Kart Wii</t>
+  </si>
+  <si>
+    <t>Left 4 Dead</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skyrim </t>
+  </si>
+  <si>
+    <t>Destiny</t>
+  </si>
+  <si>
+    <t>Super Smash Bros. Brawl</t>
+  </si>
+  <si>
+    <t>Sonic The Hedgehog</t>
+  </si>
+  <si>
+    <t>Zelda Link's Awakening</t>
+  </si>
+  <si>
+    <t>Donkey Kong 64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Last of Us </t>
+  </si>
+  <si>
+    <t>ESRB_Name</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>E 10+</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>KA</t>
   </si>
 </sst>
 </file>
@@ -192,74 +260,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -276,10 +276,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="312F2E"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="CCC4BD"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -536,17 +536,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA4E4693-5428-408F-9669-A33411403D4D}">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.44140625" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -563,7 +563,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -571,7 +571,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -579,7 +579,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -587,7 +587,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -595,7 +595,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -603,7 +603,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -611,7 +611,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -619,7 +619,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -627,7 +627,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -635,7 +635,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -643,7 +643,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -651,7 +651,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -659,192 +659,327 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15">
+        <v>5</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18">
+        <v>4</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22">
+        <v>4</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23">
+        <v>4</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25">
+        <v>3</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29">
+        <v>4</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
@@ -860,7 +995,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -874,12 +1009,12 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -887,7 +1022,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -895,7 +1030,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -903,7 +1038,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -911,7 +1046,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -919,7 +1054,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -927,7 +1062,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -935,72 +1070,72 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1018,14 +1153,14 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1042,7 +1177,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E2">
         <v>1</v>
       </c>
@@ -1056,19 +1191,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68B12098-D1F7-4CF5-AB86-01DD720B5D86}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -1082,7 +1217,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1090,7 +1225,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1098,7 +1233,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1106,7 +1241,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1114,7 +1249,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1122,7 +1257,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1130,7 +1265,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1138,7 +1273,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1146,7 +1281,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1154,52 +1289,52 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1215,7 +1350,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1223,15 +1358,63 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F04D5C45-7585-4A32-8023-6A6A92791153}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="11.109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updateing gamedb and queries
</commit_message>
<xml_diff>
--- a/GameDB.xlsx
+++ b/GameDB.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16E68955-94BA-44BF-A599-ABB0EB0C8D18}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61D70F80-67FF-4BA7-844C-3677D1240D1C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Game" sheetId="2" r:id="rId1"/>
@@ -609,8 +609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA4E4693-5428-408F-9669-A33411403D4D}">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1223,7 +1223,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1655,7 +1655,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B33D7260-6BAD-4E98-9AEB-A01C26C25698}">
   <dimension ref="B3:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3:I9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Games page in xls updated to reflect .sql
</commit_message>
<xml_diff>
--- a/GameDB.xlsx
+++ b/GameDB.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61D70F80-67FF-4BA7-844C-3677D1240D1C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B0AF7BB8-62B0-40A2-B9B0-DEE946957595}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Manufacturer" sheetId="4" r:id="rId6"/>
     <sheet name="ESRB" sheetId="6" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,10 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="85">
-  <si>
-    <t>Name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="109">
   <si>
     <t>ESRB_ID</t>
   </si>
@@ -37,42 +34,6 @@
     <t>GameID</t>
   </si>
   <si>
-    <t>Final Fantasy I</t>
-  </si>
-  <si>
-    <t>Final Fantasy IV</t>
-  </si>
-  <si>
-    <t>Final Fantasy III</t>
-  </si>
-  <si>
-    <t>Final Fantasy II</t>
-  </si>
-  <si>
-    <t>Final Fantasy V</t>
-  </si>
-  <si>
-    <t>Final Fantasy VI</t>
-  </si>
-  <si>
-    <t>Final Fantasy VII</t>
-  </si>
-  <si>
-    <t>Final Fantasy VIII</t>
-  </si>
-  <si>
-    <t>Final Fantasy IX</t>
-  </si>
-  <si>
-    <t>Final Fantasy X</t>
-  </si>
-  <si>
-    <t>Final Fantasy X-2</t>
-  </si>
-  <si>
-    <t>Final Fantasy XII</t>
-  </si>
-  <si>
     <t>GenreID</t>
   </si>
   <si>
@@ -100,9 +61,6 @@
     <t>Multiplayer</t>
   </si>
   <si>
-    <t>Online</t>
-  </si>
-  <si>
     <t>ConsoleID</t>
   </si>
   <si>
@@ -127,51 +85,6 @@
     <t>Xbox</t>
   </si>
   <si>
-    <t>Missile Command</t>
-  </si>
-  <si>
-    <t>Crash Bandicoot</t>
-  </si>
-  <si>
-    <t>Star Wars Battlefront</t>
-  </si>
-  <si>
-    <t>Halo Reach</t>
-  </si>
-  <si>
-    <t>Guitar Hero: On Tour</t>
-  </si>
-  <si>
-    <t>Monster Hunter World</t>
-  </si>
-  <si>
-    <t>Mario Kart Wii</t>
-  </si>
-  <si>
-    <t>Left 4 Dead</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Skyrim </t>
-  </si>
-  <si>
-    <t>Destiny</t>
-  </si>
-  <si>
-    <t>Super Smash Bros. Brawl</t>
-  </si>
-  <si>
-    <t>Sonic The Hedgehog</t>
-  </si>
-  <si>
-    <t>Zelda Link's Awakening</t>
-  </si>
-  <si>
-    <t>Donkey Kong 64</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Last of Us </t>
-  </si>
-  <si>
     <t>ESRB_Name</t>
   </si>
   <si>
@@ -281,6 +194,165 @@
   </si>
   <si>
     <t>Bandai</t>
+  </si>
+  <si>
+    <t>GameName</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ESRB_ID</t>
+  </si>
+  <si>
+    <t>IsOnline</t>
+  </si>
+  <si>
+    <t>'Final Fantasy I'</t>
+  </si>
+  <si>
+    <t>'Final Fantasy II'</t>
+  </si>
+  <si>
+    <t>'Final Fantasy III'</t>
+  </si>
+  <si>
+    <t>'Final Fantasy IV'</t>
+  </si>
+  <si>
+    <t>'Final Fantasy V'</t>
+  </si>
+  <si>
+    <t>'Final Fantasy VI'</t>
+  </si>
+  <si>
+    <t>'Final Fantasy VII'</t>
+  </si>
+  <si>
+    <t>'Final Fantasy VIII'</t>
+  </si>
+  <si>
+    <t>'Final FantasyIX'</t>
+  </si>
+  <si>
+    <t>'Final Fantasy X'</t>
+  </si>
+  <si>
+    <t>'Final Fantasy XI'</t>
+  </si>
+  <si>
+    <t>'Final Fantasy XII'</t>
+  </si>
+  <si>
+    <t>'Final Fantasy XIV'</t>
+  </si>
+  <si>
+    <t>'Final Fantasy XV'</t>
+  </si>
+  <si>
+    <t>'Missile Command'</t>
+  </si>
+  <si>
+    <t>'Crash Bandicoot'</t>
+  </si>
+  <si>
+    <t>'Star Wars Battlefront'</t>
+  </si>
+  <si>
+    <t>'Halo: Combat Evolved'</t>
+  </si>
+  <si>
+    <t>'Halo 2'</t>
+  </si>
+  <si>
+    <t>'Halo 3'</t>
+  </si>
+  <si>
+    <t>'Halo 3: ODST'</t>
+  </si>
+  <si>
+    <t>'Halo Reach'</t>
+  </si>
+  <si>
+    <t>'Halo 4'</t>
+  </si>
+  <si>
+    <t>'Halo 5: Guardians'</t>
+  </si>
+  <si>
+    <t>'Halo Wars'</t>
+  </si>
+  <si>
+    <t>'Halo Wars 2'</t>
+  </si>
+  <si>
+    <t>'Guitar Hero: On Tour'</t>
+  </si>
+  <si>
+    <t>'Monster Hunter World'</t>
+  </si>
+  <si>
+    <t>'Mario Kart 64'</t>
+  </si>
+  <si>
+    <t>'Mario Kart Wii'</t>
+  </si>
+  <si>
+    <t>'Left 4 Dead'</t>
+  </si>
+  <si>
+    <t>'Elder Scrolls: Arena'</t>
+  </si>
+  <si>
+    <t>'Elder Scrolls II: Daggerfall'</t>
+  </si>
+  <si>
+    <t>'Elder Scrolls III: Marrowind'</t>
+  </si>
+  <si>
+    <t>'Elder Scrolls IV: Oblivion'</t>
+  </si>
+  <si>
+    <t>'Elder Scrolls V: Skyrim'</t>
+  </si>
+  <si>
+    <t>'Elder Scrolls Online'</t>
+  </si>
+  <si>
+    <t>'Destiny'</t>
+  </si>
+  <si>
+    <t>'Destiny 2'</t>
+  </si>
+  <si>
+    <t>'Super Smash Bros. Brawl'</t>
+  </si>
+  <si>
+    <t>'Sonic The Hedgehog'</t>
+  </si>
+  <si>
+    <t>'Legend of Zelda'</t>
+  </si>
+  <si>
+    <t>'Legend of Zelda: Ocarina of Time'</t>
+  </si>
+  <si>
+    <t>'Legend of Zelda: Majoras Mask'</t>
+  </si>
+  <si>
+    <t>'Legend of Zelda Links Awakening'</t>
+  </si>
+  <si>
+    <t>'Donkey Kong 64'</t>
+  </si>
+  <si>
+    <t>'Mario 64'</t>
+  </si>
+  <si>
+    <t>'Last of Us'</t>
+  </si>
+  <si>
+    <t>'Crazy Taxi'</t>
+  </si>
+  <si>
+    <t>'Civilizations'</t>
   </si>
 </sst>
 </file>
@@ -610,7 +682,7 @@
   <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:A29"/>
+      <selection sqref="A1:E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -621,19 +693,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="D1" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="E1" t="s">
-        <v>24</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -641,7 +713,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>59</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -649,7 +730,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>60</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -657,7 +747,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>61</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -665,7 +764,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>62</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -673,7 +781,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>63</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -681,7 +798,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>64</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -689,7 +815,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>65</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -697,7 +832,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>66</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -705,7 +849,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>67</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -713,7 +866,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>68</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -721,7 +883,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>69</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -729,7 +900,16 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>70</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -737,13 +917,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -751,10 +934,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
+        <v>72</v>
       </c>
       <c r="C15">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -765,10 +951,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>35</v>
+        <v>73</v>
       </c>
       <c r="C16">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -778,19 +967,34 @@
       <c r="A17">
         <v>16</v>
       </c>
+      <c r="B17" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17">
+        <v>5</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>36</v>
+        <v>75</v>
       </c>
       <c r="C18">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
       </c>
       <c r="E18">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -798,13 +1002,16 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>37</v>
+        <v>76</v>
       </c>
       <c r="C19">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -812,10 +1019,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>77</v>
       </c>
       <c r="C20">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
       </c>
       <c r="E20">
         <v>1</v>
@@ -826,9 +1036,12 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>39</v>
+        <v>78</v>
       </c>
       <c r="C21">
+        <v>4</v>
+      </c>
+      <c r="D21">
         <v>1</v>
       </c>
       <c r="E21">
@@ -840,10 +1053,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>79</v>
       </c>
       <c r="C22">
         <v>4</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
       </c>
       <c r="E22">
         <v>1</v>
@@ -854,13 +1070,16 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="C23">
         <v>4</v>
       </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
       <c r="E23">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -868,10 +1087,13 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>42</v>
+        <v>81</v>
       </c>
       <c r="C24">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
       </c>
       <c r="E24">
         <v>1</v>
@@ -882,10 +1104,13 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>43</v>
+        <v>82</v>
       </c>
       <c r="C25">
         <v>3</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
       </c>
       <c r="E25">
         <v>1</v>
@@ -896,13 +1121,16 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>44</v>
+        <v>83</v>
       </c>
       <c r="C26">
+        <v>3</v>
+      </c>
+      <c r="D26">
         <v>1</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -910,13 +1138,16 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>45</v>
+        <v>84</v>
       </c>
       <c r="C27">
+        <v>3</v>
+      </c>
+      <c r="D27">
         <v>1</v>
       </c>
       <c r="E27">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -924,9 +1155,12 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>46</v>
+        <v>85</v>
       </c>
       <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28">
         <v>1</v>
       </c>
       <c r="E28">
@@ -938,123 +1172,390 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>47</v>
+        <v>86</v>
       </c>
       <c r="C29">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
       </c>
       <c r="E29">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
+      <c r="B30" t="s">
+        <v>87</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
+      <c r="B31" t="s">
+        <v>88</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>89</v>
+      </c>
+      <c r="C32">
+        <v>4</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>90</v>
+      </c>
+      <c r="C33">
+        <v>4</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>91</v>
+      </c>
+      <c r="C34">
+        <v>4</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>92</v>
+      </c>
+      <c r="C35">
+        <v>4</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>93</v>
+      </c>
+      <c r="C36">
+        <v>4</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>94</v>
+      </c>
+      <c r="C37">
+        <v>4</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>95</v>
+      </c>
+      <c r="C38">
+        <v>4</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>96</v>
+      </c>
+      <c r="C39">
+        <v>3</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>97</v>
+      </c>
+      <c r="C40">
+        <v>3</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>98</v>
+      </c>
+      <c r="C41">
+        <v>3</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>99</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>100</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>101</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>102</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>103</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>104</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>105</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>106</v>
+      </c>
+      <c r="C49">
+        <v>4</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>107</v>
+      </c>
+      <c r="C50">
+        <v>3</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>108</v>
+      </c>
+      <c r="C51">
+        <v>2</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1089,10 +1590,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1100,7 +1601,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1108,7 +1609,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1116,7 +1617,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1124,7 +1625,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1132,7 +1633,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1140,7 +1641,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1235,19 +1736,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="D1" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="E1" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1278,13 +1779,13 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
         <v>25</v>
       </c>
-      <c r="B1" t="s">
-        <v>54</v>
-      </c>
       <c r="C1" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1295,7 +1796,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="H2" t="str">
         <f>"INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('"&amp;A2&amp;"','"&amp;B2&amp;"','"&amp;C2&amp;"')"</f>
@@ -1310,7 +1811,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>56</v>
+        <v>27</v>
       </c>
       <c r="H3" t="str">
         <f t="shared" ref="H3:H23" si="0">"INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('"&amp;A3&amp;"','"&amp;B3&amp;"','"&amp;C3&amp;"')"</f>
@@ -1325,7 +1826,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>57</v>
+        <v>28</v>
       </c>
       <c r="H4" t="str">
         <f t="shared" si="0"/>
@@ -1340,7 +1841,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>58</v>
+        <v>29</v>
       </c>
       <c r="H5" t="str">
         <f t="shared" si="0"/>
@@ -1355,7 +1856,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="H6" t="str">
         <f t="shared" si="0"/>
@@ -1370,7 +1871,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>60</v>
+        <v>31</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" si="0"/>
@@ -1385,7 +1886,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="H8" t="str">
         <f t="shared" si="0"/>
@@ -1400,7 +1901,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>61</v>
+        <v>32</v>
       </c>
       <c r="H9" t="str">
         <f t="shared" si="0"/>
@@ -1415,7 +1916,7 @@
         <v>3</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>62</v>
+        <v>33</v>
       </c>
       <c r="H10" t="str">
         <f t="shared" si="0"/>
@@ -1430,7 +1931,7 @@
         <v>5</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="H11" t="str">
         <f t="shared" si="0"/>
@@ -1445,7 +1946,7 @@
         <v>5</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>64</v>
+        <v>35</v>
       </c>
       <c r="H12" t="str">
         <f t="shared" si="0"/>
@@ -1460,7 +1961,7 @@
         <v>5</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>65</v>
+        <v>36</v>
       </c>
       <c r="H13" t="str">
         <f t="shared" si="0"/>
@@ -1475,7 +1976,7 @@
         <v>2</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>66</v>
+        <v>37</v>
       </c>
       <c r="H14" t="str">
         <f t="shared" si="0"/>
@@ -1490,7 +1991,7 @@
         <v>2</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>67</v>
+        <v>38</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="0"/>
@@ -1505,7 +2006,7 @@
         <v>2</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
       <c r="H16" t="str">
         <f t="shared" si="0"/>
@@ -1520,7 +2021,7 @@
         <v>2</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="H17" t="str">
         <f t="shared" si="0"/>
@@ -1535,7 +2036,7 @@
         <v>2</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>70</v>
+        <v>41</v>
       </c>
       <c r="H18" t="str">
         <f t="shared" si="0"/>
@@ -1550,7 +2051,7 @@
         <v>1</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>71</v>
+        <v>42</v>
       </c>
       <c r="H19" t="str">
         <f t="shared" si="0"/>
@@ -1565,7 +2066,7 @@
         <v>2</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>72</v>
+        <v>43</v>
       </c>
       <c r="H20" t="str">
         <f t="shared" si="0"/>
@@ -1580,7 +2081,7 @@
         <v>2</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>73</v>
+        <v>44</v>
       </c>
       <c r="H21" t="str">
         <f t="shared" si="0"/>
@@ -1595,7 +2096,7 @@
         <v>2</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>74</v>
+        <v>45</v>
       </c>
       <c r="H22" t="str">
         <f t="shared" si="0"/>
@@ -1610,7 +2111,7 @@
         <v>2</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="H23" t="str">
         <f t="shared" si="0"/>
@@ -1625,7 +2126,7 @@
         <v>2</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>76</v>
+        <v>47</v>
       </c>
       <c r="H24" t="str">
         <f>"INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('"&amp;A24&amp;"','"&amp;B24&amp;"','"&amp;C24&amp;"')"</f>
@@ -1640,10 +2141,10 @@
         <v>6</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>77</v>
+        <v>48</v>
       </c>
       <c r="H25" t="s">
-        <v>78</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1663,10 +2164,10 @@
   <sheetData>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>79</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
@@ -1674,7 +2175,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>80</v>
+        <v>51</v>
       </c>
       <c r="I4" t="str">
         <f>"INSERT @Manufacturer (ManufacturerID, ManufacturerName) VALUES ('"&amp;B4&amp;"','"&amp;C4&amp;"')"</f>
@@ -1686,7 +2187,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>81</v>
+        <v>52</v>
       </c>
       <c r="I5" t="str">
         <f t="shared" ref="I5:I9" si="0">"INSERT @Manufacturer (ManufacturerID, ManufacturerName) VALUES ('"&amp;B5&amp;"','"&amp;C5&amp;"')"</f>
@@ -1698,7 +2199,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>82</v>
+        <v>53</v>
       </c>
       <c r="I6" t="str">
         <f t="shared" si="0"/>
@@ -1710,7 +2211,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>83</v>
+        <v>54</v>
       </c>
       <c r="I7" t="str">
         <f t="shared" si="0"/>
@@ -1722,7 +2223,7 @@
         <v>5</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="I8" t="str">
         <f t="shared" si="0"/>
@@ -1734,7 +2235,7 @@
         <v>6</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>84</v>
+        <v>55</v>
       </c>
       <c r="I9" t="str">
         <f t="shared" si="0"/>
@@ -1761,10 +2262,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>48</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1772,7 +2273,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1780,7 +2281,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1788,7 +2289,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1796,7 +2297,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1804,7 +2305,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
maybe this shold have been separate .xls?  or maybe did csv instead? (easier to Diff, being a text file)
</commit_message>
<xml_diff>
--- a/GameDB.xlsx
+++ b/GameDB.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B0AF7BB8-62B0-40A2-B9B0-DEE946957595}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{3252BEB3-1E7D-434F-8FF2-62A178ADA2C0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Game" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="117">
   <si>
     <t>ESRB_ID</t>
   </si>
@@ -37,27 +37,6 @@
     <t>GenreID</t>
   </si>
   <si>
-    <t>Genre</t>
-  </si>
-  <si>
-    <t>Role Playing Game</t>
-  </si>
-  <si>
-    <t>Real Time Strategy</t>
-  </si>
-  <si>
-    <t>Turn Based Strategy</t>
-  </si>
-  <si>
-    <t>First Person Shooter</t>
-  </si>
-  <si>
-    <t>Exploration</t>
-  </si>
-  <si>
-    <t>Sandbox</t>
-  </si>
-  <si>
     <t>Multiplayer</t>
   </si>
   <si>
@@ -353,6 +332,51 @@
   </si>
   <si>
     <t>'Civilizations'</t>
+  </si>
+  <si>
+    <t>GameGenreID</t>
+  </si>
+  <si>
+    <t>'Role Playing Game'</t>
+  </si>
+  <si>
+    <t>'Real Time Strategy'</t>
+  </si>
+  <si>
+    <t>'Turn Based Strategy'</t>
+  </si>
+  <si>
+    <t>'First Person Shooter'</t>
+  </si>
+  <si>
+    <t>'Exploration'</t>
+  </si>
+  <si>
+    <t>'Sandbox'</t>
+  </si>
+  <si>
+    <t>'Platformer'</t>
+  </si>
+  <si>
+    <t>'Music'</t>
+  </si>
+  <si>
+    <t>'Third Person Shooter'</t>
+  </si>
+  <si>
+    <t>'Puzzle'</t>
+  </si>
+  <si>
+    <t>'Sports'</t>
+  </si>
+  <si>
+    <t>'Racing'</t>
+  </si>
+  <si>
+    <t>'Fighting'</t>
+  </si>
+  <si>
+    <t>GenreName</t>
   </si>
 </sst>
 </file>
@@ -681,8 +705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA4E4693-5428-408F-9669-A33411403D4D}">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E51"/>
+    <sheetView topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="B51" sqref="B2:B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,16 +720,16 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -713,7 +737,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -730,7 +754,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C3">
         <v>3</v>
@@ -747,7 +771,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -764,7 +788,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -781,7 +805,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -798,7 +822,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -815,7 +839,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C8">
         <v>3</v>
@@ -832,7 +856,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C9">
         <v>3</v>
@@ -849,7 +873,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C10">
         <v>3</v>
@@ -866,7 +890,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C11">
         <v>3</v>
@@ -883,7 +907,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C12">
         <v>3</v>
@@ -900,7 +924,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="C13">
         <v>3</v>
@@ -917,7 +941,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C14">
         <v>3</v>
@@ -934,7 +958,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C15">
         <v>3</v>
@@ -951,7 +975,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -968,7 +992,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C17">
         <v>5</v>
@@ -985,7 +1009,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C18">
         <v>3</v>
@@ -1002,7 +1026,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C19">
         <v>4</v>
@@ -1019,7 +1043,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C20">
         <v>4</v>
@@ -1036,7 +1060,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C21">
         <v>4</v>
@@ -1053,7 +1077,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C22">
         <v>4</v>
@@ -1070,7 +1094,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="C23">
         <v>4</v>
@@ -1087,7 +1111,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C24">
         <v>4</v>
@@ -1104,7 +1128,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C25">
         <v>3</v>
@@ -1121,7 +1145,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C26">
         <v>3</v>
@@ -1138,7 +1162,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C27">
         <v>3</v>
@@ -1155,7 +1179,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C28">
         <v>2</v>
@@ -1172,7 +1196,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C29">
         <v>3</v>
@@ -1189,7 +1213,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -1206,7 +1230,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -1223,7 +1247,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C32">
         <v>4</v>
@@ -1240,7 +1264,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C33">
         <v>4</v>
@@ -1257,7 +1281,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="C34">
         <v>4</v>
@@ -1274,7 +1298,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="C35">
         <v>4</v>
@@ -1291,7 +1315,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C36">
         <v>4</v>
@@ -1308,7 +1332,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="C37">
         <v>4</v>
@@ -1325,7 +1349,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="C38">
         <v>4</v>
@@ -1342,7 +1366,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="C39">
         <v>3</v>
@@ -1359,7 +1383,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="C40">
         <v>3</v>
@@ -1376,7 +1400,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="C41">
         <v>3</v>
@@ -1393,7 +1417,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="C42">
         <v>1</v>
@@ -1410,7 +1434,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="C43">
         <v>1</v>
@@ -1427,7 +1451,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="C44">
         <v>1</v>
@@ -1444,7 +1468,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="C45">
         <v>1</v>
@@ -1461,7 +1485,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="C46">
         <v>1</v>
@@ -1478,7 +1502,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="C47">
         <v>1</v>
@@ -1495,7 +1519,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="C48">
         <v>1</v>
@@ -1512,7 +1536,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="C49">
         <v>4</v>
@@ -1529,7 +1553,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="C50">
         <v>3</v>
@@ -1546,7 +1570,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="C51">
         <v>2</v>
@@ -1565,27 +1589,623 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7">
+        <v>6</v>
+      </c>
+      <c r="F7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8">
+        <v>7</v>
+      </c>
+      <c r="F8" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9">
+        <v>8</v>
+      </c>
+      <c r="F9" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10">
+        <v>9</v>
+      </c>
+      <c r="F10" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11">
+        <v>10</v>
+      </c>
+      <c r="F11" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>11</v>
+      </c>
+      <c r="D12" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12">
+        <v>11</v>
+      </c>
+      <c r="F12" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>12</v>
+      </c>
+      <c r="D13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13">
+        <v>12</v>
+      </c>
+      <c r="F13" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>13</v>
+      </c>
+      <c r="D14" t="s">
+        <v>64</v>
+      </c>
+      <c r="E14">
+        <v>13</v>
+      </c>
+      <c r="F14" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>14</v>
+      </c>
+      <c r="D15" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>15</v>
+      </c>
+      <c r="D16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>7</v>
+      </c>
+      <c r="C17">
+        <v>16</v>
+      </c>
+      <c r="D17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>9</v>
+      </c>
+      <c r="C18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>17</v>
+      </c>
+      <c r="D19" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>4</v>
+      </c>
+      <c r="C20">
+        <v>18</v>
+      </c>
+      <c r="D20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>4</v>
+      </c>
+      <c r="C21">
+        <v>19</v>
+      </c>
+      <c r="D21" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>4</v>
+      </c>
+      <c r="C22">
+        <v>20</v>
+      </c>
+      <c r="D22" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="C23">
+        <v>21</v>
+      </c>
+      <c r="D23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="C24">
+        <v>22</v>
+      </c>
+      <c r="D24" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>4</v>
+      </c>
+      <c r="C25">
+        <v>23</v>
+      </c>
+      <c r="D25" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>4</v>
+      </c>
+      <c r="C26">
+        <v>24</v>
+      </c>
+      <c r="D26" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <v>25</v>
+      </c>
+      <c r="D27" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <v>26</v>
+      </c>
+      <c r="D28" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <v>27</v>
+      </c>
+      <c r="D29" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C30">
+        <v>28</v>
+      </c>
+      <c r="D30" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C31">
+        <v>29</v>
+      </c>
+      <c r="D31" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C32">
+        <v>30</v>
+      </c>
+      <c r="D32" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C33">
+        <v>31</v>
+      </c>
+      <c r="D33" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <v>32</v>
+      </c>
+      <c r="D34" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>33</v>
+      </c>
+      <c r="D35" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <v>34</v>
+      </c>
+      <c r="D36" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37">
+        <v>35</v>
+      </c>
+      <c r="D37" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38">
+        <v>36</v>
+      </c>
+      <c r="D38" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39">
+        <v>37</v>
+      </c>
+      <c r="D39" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C40">
+        <v>38</v>
+      </c>
+      <c r="D40" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C41">
+        <v>39</v>
+      </c>
+      <c r="D41" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C42">
+        <v>40</v>
+      </c>
+      <c r="D42" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C43">
+        <v>41</v>
+      </c>
+      <c r="D43" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C44">
+        <v>42</v>
+      </c>
+      <c r="D44" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C45">
+        <v>43</v>
+      </c>
+      <c r="D45" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C46">
+        <v>44</v>
+      </c>
+      <c r="D46" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C47">
+        <v>45</v>
+      </c>
+      <c r="D47" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C48">
+        <v>46</v>
+      </c>
+      <c r="D48" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C49">
+        <v>47</v>
+      </c>
+      <c r="D49" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C50">
+        <v>48</v>
+      </c>
+      <c r="D50" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C51">
+        <v>49</v>
+      </c>
+      <c r="D51" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C52">
+        <v>50</v>
+      </c>
+      <c r="D52" t="s">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EF5F056-BA29-4194-9E5D-8390E9600CC5}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1593,7 +2213,7 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1601,7 +2221,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1609,7 +2229,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1617,7 +2237,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1625,7 +2245,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1633,7 +2253,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1641,77 +2261,63 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
+      <c r="B8" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
+      <c r="B9" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
+      <c r="B10" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
+      <c r="B11" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
+      <c r="B12" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
+      <c r="B13" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>20</v>
+      <c r="B14" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -1739,16 +2345,16 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D1" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="E1" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1779,13 +2385,13 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1796,7 +2402,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="H2" t="str">
         <f>"INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('"&amp;A2&amp;"','"&amp;B2&amp;"','"&amp;C2&amp;"')"</f>
@@ -1811,7 +2417,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="H3" t="str">
         <f t="shared" ref="H3:H23" si="0">"INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('"&amp;A3&amp;"','"&amp;B3&amp;"','"&amp;C3&amp;"')"</f>
@@ -1826,7 +2432,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="H4" t="str">
         <f t="shared" si="0"/>
@@ -1841,7 +2447,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="H5" t="str">
         <f t="shared" si="0"/>
@@ -1856,7 +2462,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="H6" t="str">
         <f t="shared" si="0"/>
@@ -1871,7 +2477,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" si="0"/>
@@ -1886,7 +2492,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H8" t="str">
         <f t="shared" si="0"/>
@@ -1901,7 +2507,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="H9" t="str">
         <f t="shared" si="0"/>
@@ -1916,7 +2522,7 @@
         <v>3</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="H10" t="str">
         <f t="shared" si="0"/>
@@ -1931,7 +2537,7 @@
         <v>5</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="H11" t="str">
         <f t="shared" si="0"/>
@@ -1946,7 +2552,7 @@
         <v>5</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="H12" t="str">
         <f t="shared" si="0"/>
@@ -1961,7 +2567,7 @@
         <v>5</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="H13" t="str">
         <f t="shared" si="0"/>
@@ -1976,7 +2582,7 @@
         <v>2</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H14" t="str">
         <f t="shared" si="0"/>
@@ -1991,7 +2597,7 @@
         <v>2</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="0"/>
@@ -2006,7 +2612,7 @@
         <v>2</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="H16" t="str">
         <f t="shared" si="0"/>
@@ -2021,7 +2627,7 @@
         <v>2</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="H17" t="str">
         <f t="shared" si="0"/>
@@ -2036,7 +2642,7 @@
         <v>2</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="H18" t="str">
         <f t="shared" si="0"/>
@@ -2051,7 +2657,7 @@
         <v>1</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="H19" t="str">
         <f t="shared" si="0"/>
@@ -2066,7 +2672,7 @@
         <v>2</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="H20" t="str">
         <f t="shared" si="0"/>
@@ -2081,7 +2687,7 @@
         <v>2</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="H21" t="str">
         <f t="shared" si="0"/>
@@ -2096,7 +2702,7 @@
         <v>2</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="H22" t="str">
         <f t="shared" si="0"/>
@@ -2111,7 +2717,7 @@
         <v>2</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="H23" t="str">
         <f t="shared" si="0"/>
@@ -2126,7 +2732,7 @@
         <v>2</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="H24" t="str">
         <f>"INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('"&amp;A24&amp;"','"&amp;B24&amp;"','"&amp;C24&amp;"')"</f>
@@ -2141,10 +2747,10 @@
         <v>6</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="H25" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -2164,10 +2770,10 @@
   <sheetData>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
@@ -2175,7 +2781,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="I4" t="str">
         <f>"INSERT @Manufacturer (ManufacturerID, ManufacturerName) VALUES ('"&amp;B4&amp;"','"&amp;C4&amp;"')"</f>
@@ -2187,7 +2793,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="I5" t="str">
         <f t="shared" ref="I5:I9" si="0">"INSERT @Manufacturer (ManufacturerID, ManufacturerName) VALUES ('"&amp;B5&amp;"','"&amp;C5&amp;"')"</f>
@@ -2199,7 +2805,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="I6" t="str">
         <f t="shared" si="0"/>
@@ -2211,7 +2817,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="I7" t="str">
         <f t="shared" si="0"/>
@@ -2223,7 +2829,7 @@
         <v>5</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="I8" t="str">
         <f t="shared" si="0"/>
@@ -2235,7 +2841,7 @@
         <v>6</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="I9" t="str">
         <f t="shared" si="0"/>
@@ -2265,7 +2871,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2273,7 +2879,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2281,7 +2887,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2289,7 +2895,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2297,7 +2903,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2305,7 +2911,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on catalogue table
</commit_message>
<xml_diff>
--- a/GameDB.xlsx
+++ b/GameDB.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{3252BEB3-1E7D-434F-8FF2-62A178ADA2C0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8EA64400-2C76-4C12-BA04-BE1C7D02B5BB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Game" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="117">
   <si>
     <t>ESRB_ID</t>
   </si>
@@ -43,9 +43,6 @@
     <t>ConsoleID</t>
   </si>
   <si>
-    <t>Rating</t>
-  </si>
-  <si>
     <t>PurchaseDate</t>
   </si>
   <si>
@@ -377,6 +374,9 @@
   </si>
   <si>
     <t>GenreName</t>
+  </si>
+  <si>
+    <t>CatalogueID</t>
   </si>
 </sst>
 </file>
@@ -406,10 +406,19 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -418,11 +427,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -720,16 +730,16 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" t="s">
         <v>49</v>
-      </c>
-      <c r="C1" t="s">
-        <v>50</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -737,7 +747,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -754,7 +764,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C3">
         <v>3</v>
@@ -771,7 +781,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -788,7 +798,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -805,7 +815,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -822,7 +832,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -839,7 +849,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C8">
         <v>3</v>
@@ -856,7 +866,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C9">
         <v>3</v>
@@ -873,7 +883,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C10">
         <v>3</v>
@@ -890,7 +900,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C11">
         <v>3</v>
@@ -907,7 +917,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C12">
         <v>3</v>
@@ -924,7 +934,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C13">
         <v>3</v>
@@ -941,7 +951,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C14">
         <v>3</v>
@@ -958,7 +968,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C15">
         <v>3</v>
@@ -975,7 +985,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -992,7 +1002,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C17">
         <v>5</v>
@@ -1009,7 +1019,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C18">
         <v>3</v>
@@ -1026,7 +1036,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C19">
         <v>4</v>
@@ -1043,7 +1053,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C20">
         <v>4</v>
@@ -1060,7 +1070,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C21">
         <v>4</v>
@@ -1077,7 +1087,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C22">
         <v>4</v>
@@ -1094,7 +1104,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C23">
         <v>4</v>
@@ -1111,7 +1121,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C24">
         <v>4</v>
@@ -1128,7 +1138,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C25">
         <v>3</v>
@@ -1145,7 +1155,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C26">
         <v>3</v>
@@ -1162,7 +1172,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C27">
         <v>3</v>
@@ -1179,7 +1189,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C28">
         <v>2</v>
@@ -1196,7 +1206,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C29">
         <v>3</v>
@@ -1213,7 +1223,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -1230,7 +1240,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -1247,7 +1257,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C32">
         <v>4</v>
@@ -1264,7 +1274,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C33">
         <v>4</v>
@@ -1281,7 +1291,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C34">
         <v>4</v>
@@ -1298,7 +1308,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C35">
         <v>4</v>
@@ -1315,7 +1325,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C36">
         <v>4</v>
@@ -1332,7 +1342,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C37">
         <v>4</v>
@@ -1349,7 +1359,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C38">
         <v>4</v>
@@ -1366,7 +1376,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C39">
         <v>3</v>
@@ -1383,7 +1393,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C40">
         <v>3</v>
@@ -1400,7 +1410,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C41">
         <v>3</v>
@@ -1417,7 +1427,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C42">
         <v>1</v>
@@ -1434,7 +1444,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C43">
         <v>1</v>
@@ -1451,7 +1461,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C44">
         <v>1</v>
@@ -1468,7 +1478,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C45">
         <v>1</v>
@@ -1485,7 +1495,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C46">
         <v>1</v>
@@ -1502,7 +1512,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C47">
         <v>1</v>
@@ -1519,7 +1529,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C48">
         <v>1</v>
@@ -1536,7 +1546,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C49">
         <v>4</v>
@@ -1553,7 +1563,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C50">
         <v>3</v>
@@ -1570,7 +1580,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C51">
         <v>2</v>
@@ -1591,7 +1601,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -1604,7 +1614,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -1624,13 +1634,13 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1641,13 +1651,13 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E3">
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1658,13 +1668,13 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E4">
         <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1675,13 +1685,13 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E5">
         <v>4</v>
       </c>
       <c r="F5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1692,13 +1702,13 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E6">
         <v>5</v>
       </c>
       <c r="F6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1709,13 +1719,13 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E7">
         <v>6</v>
       </c>
       <c r="F7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1726,13 +1736,13 @@
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E8">
         <v>7</v>
       </c>
       <c r="F8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1743,13 +1753,13 @@
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E9">
         <v>8</v>
       </c>
       <c r="F9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1760,13 +1770,13 @@
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E10">
         <v>9</v>
       </c>
       <c r="F10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1777,13 +1787,13 @@
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E11">
         <v>10</v>
       </c>
       <c r="F11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1794,13 +1804,13 @@
         <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E12">
         <v>11</v>
       </c>
       <c r="F12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1811,13 +1821,13 @@
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E13">
         <v>12</v>
       </c>
       <c r="F13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1828,13 +1838,13 @@
         <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E14">
         <v>13</v>
       </c>
       <c r="F14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1845,7 +1855,7 @@
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1853,7 +1863,7 @@
         <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
@@ -1864,7 +1874,7 @@
         <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
@@ -1883,7 +1893,7 @@
         <v>17</v>
       </c>
       <c r="D19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
@@ -1894,7 +1904,7 @@
         <v>18</v>
       </c>
       <c r="D20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
@@ -1905,7 +1915,7 @@
         <v>19</v>
       </c>
       <c r="D21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
@@ -1916,7 +1926,7 @@
         <v>20</v>
       </c>
       <c r="D22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
@@ -1927,7 +1937,7 @@
         <v>21</v>
       </c>
       <c r="D23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
@@ -1938,7 +1948,7 @@
         <v>22</v>
       </c>
       <c r="D24" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
@@ -1949,7 +1959,7 @@
         <v>23</v>
       </c>
       <c r="D25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
@@ -1960,7 +1970,7 @@
         <v>24</v>
       </c>
       <c r="D26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
@@ -1968,7 +1978,7 @@
         <v>25</v>
       </c>
       <c r="D27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
@@ -1976,7 +1986,7 @@
         <v>26</v>
       </c>
       <c r="D28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
@@ -1984,7 +1994,7 @@
         <v>27</v>
       </c>
       <c r="D29" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
@@ -1992,7 +2002,7 @@
         <v>28</v>
       </c>
       <c r="D30" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
@@ -2000,7 +2010,7 @@
         <v>29</v>
       </c>
       <c r="D31" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
@@ -2008,7 +2018,7 @@
         <v>30</v>
       </c>
       <c r="D32" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
@@ -2016,7 +2026,7 @@
         <v>31</v>
       </c>
       <c r="D33" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
@@ -2027,7 +2037,7 @@
         <v>32</v>
       </c>
       <c r="D34" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
@@ -2038,7 +2048,7 @@
         <v>33</v>
       </c>
       <c r="D35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
@@ -2049,7 +2059,7 @@
         <v>34</v>
       </c>
       <c r="D36" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
@@ -2060,7 +2070,7 @@
         <v>35</v>
       </c>
       <c r="D37" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
@@ -2071,7 +2081,7 @@
         <v>36</v>
       </c>
       <c r="D38" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
@@ -2082,7 +2092,7 @@
         <v>37</v>
       </c>
       <c r="D39" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
@@ -2090,7 +2100,7 @@
         <v>38</v>
       </c>
       <c r="D40" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.25">
@@ -2098,7 +2108,7 @@
         <v>39</v>
       </c>
       <c r="D41" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.25">
@@ -2106,7 +2116,7 @@
         <v>40</v>
       </c>
       <c r="D42" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.25">
@@ -2114,7 +2124,7 @@
         <v>41</v>
       </c>
       <c r="D43" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.25">
@@ -2122,7 +2132,7 @@
         <v>42</v>
       </c>
       <c r="D44" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.25">
@@ -2130,7 +2140,7 @@
         <v>43</v>
       </c>
       <c r="D45" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.25">
@@ -2138,7 +2148,7 @@
         <v>44</v>
       </c>
       <c r="D46" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.25">
@@ -2146,7 +2156,7 @@
         <v>45</v>
       </c>
       <c r="D47" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.25">
@@ -2154,7 +2164,7 @@
         <v>46</v>
       </c>
       <c r="D48" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="49" spans="3:4" x14ac:dyDescent="0.25">
@@ -2162,7 +2172,7 @@
         <v>47</v>
       </c>
       <c r="D49" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="50" spans="3:4" x14ac:dyDescent="0.25">
@@ -2170,7 +2180,7 @@
         <v>48</v>
       </c>
       <c r="D50" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="51" spans="3:4" x14ac:dyDescent="0.25">
@@ -2178,7 +2188,7 @@
         <v>49</v>
       </c>
       <c r="D51" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="52" spans="3:4" x14ac:dyDescent="0.25">
@@ -2186,7 +2196,7 @@
         <v>50</v>
       </c>
       <c r="D52" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -2213,7 +2223,7 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2221,7 +2231,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2229,7 +2239,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2237,7 +2247,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2245,7 +2255,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2253,7 +2263,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -2261,7 +2271,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -2269,7 +2279,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -2277,7 +2287,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -2285,7 +2295,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -2293,7 +2303,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -2301,7 +2311,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -2309,7 +2319,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -2317,7 +2327,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -2327,39 +2337,292 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB34F316-239A-4088-B766-2DFF3070945E}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>116</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E2">
-        <v>1</v>
+      <c r="H1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E2" s="2">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H17" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H18" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H19" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H21" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H22" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H24" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H25" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H26" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H27" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H28" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="29" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H29" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="30" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H30" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H31" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H32" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="33" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H33" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="34" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H34" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="35" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H35" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="36" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H36" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="37" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H37" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="38" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H38" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="39" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H39" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="40" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H40" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="41" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H41" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="42" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H42" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="43" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H43" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="44" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H44" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="45" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H45" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="46" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H46" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="47" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H47" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="48" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H48" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="49" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H49" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="50" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H50" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="51" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H51" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -2388,10 +2651,10 @@
         <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -2402,7 +2665,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H2" t="str">
         <f>"INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('"&amp;A2&amp;"','"&amp;B2&amp;"','"&amp;C2&amp;"')"</f>
@@ -2417,7 +2680,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H3" t="str">
         <f t="shared" ref="H3:H23" si="0">"INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('"&amp;A3&amp;"','"&amp;B3&amp;"','"&amp;C3&amp;"')"</f>
@@ -2432,7 +2695,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H4" t="str">
         <f t="shared" si="0"/>
@@ -2447,7 +2710,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H5" t="str">
         <f t="shared" si="0"/>
@@ -2462,7 +2725,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H6" t="str">
         <f t="shared" si="0"/>
@@ -2477,7 +2740,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" si="0"/>
@@ -2492,7 +2755,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H8" t="str">
         <f t="shared" si="0"/>
@@ -2507,7 +2770,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H9" t="str">
         <f t="shared" si="0"/>
@@ -2522,7 +2785,7 @@
         <v>3</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H10" t="str">
         <f t="shared" si="0"/>
@@ -2537,7 +2800,7 @@
         <v>5</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H11" t="str">
         <f t="shared" si="0"/>
@@ -2552,7 +2815,7 @@
         <v>5</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H12" t="str">
         <f t="shared" si="0"/>
@@ -2567,7 +2830,7 @@
         <v>5</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H13" t="str">
         <f t="shared" si="0"/>
@@ -2582,7 +2845,7 @@
         <v>2</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H14" t="str">
         <f t="shared" si="0"/>
@@ -2597,7 +2860,7 @@
         <v>2</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="0"/>
@@ -2612,7 +2875,7 @@
         <v>2</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H16" t="str">
         <f t="shared" si="0"/>
@@ -2627,7 +2890,7 @@
         <v>2</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H17" t="str">
         <f t="shared" si="0"/>
@@ -2642,7 +2905,7 @@
         <v>2</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H18" t="str">
         <f t="shared" si="0"/>
@@ -2657,7 +2920,7 @@
         <v>1</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H19" t="str">
         <f t="shared" si="0"/>
@@ -2672,7 +2935,7 @@
         <v>2</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H20" t="str">
         <f t="shared" si="0"/>
@@ -2687,7 +2950,7 @@
         <v>2</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H21" t="str">
         <f t="shared" si="0"/>
@@ -2702,7 +2965,7 @@
         <v>2</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H22" t="str">
         <f t="shared" si="0"/>
@@ -2717,7 +2980,7 @@
         <v>2</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H23" t="str">
         <f t="shared" si="0"/>
@@ -2732,7 +2995,7 @@
         <v>2</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H24" t="str">
         <f>"INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('"&amp;A24&amp;"','"&amp;B24&amp;"','"&amp;C24&amp;"')"</f>
@@ -2747,10 +3010,10 @@
         <v>6</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H25" t="s">
         <v>41</v>
-      </c>
-      <c r="H25" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -2770,10 +3033,10 @@
   <sheetData>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
@@ -2781,7 +3044,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I4" t="str">
         <f>"INSERT @Manufacturer (ManufacturerID, ManufacturerName) VALUES ('"&amp;B4&amp;"','"&amp;C4&amp;"')"</f>
@@ -2793,7 +3056,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I5" t="str">
         <f t="shared" ref="I5:I9" si="0">"INSERT @Manufacturer (ManufacturerID, ManufacturerName) VALUES ('"&amp;B5&amp;"','"&amp;C5&amp;"')"</f>
@@ -2805,7 +3068,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I6" t="str">
         <f t="shared" si="0"/>
@@ -2817,7 +3080,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I7" t="str">
         <f t="shared" si="0"/>
@@ -2829,7 +3092,7 @@
         <v>5</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I8" t="str">
         <f t="shared" si="0"/>
@@ -2841,7 +3104,7 @@
         <v>6</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I9" t="str">
         <f t="shared" si="0"/>
@@ -2871,7 +3134,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2879,7 +3142,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2887,7 +3150,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2895,7 +3158,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2903,7 +3166,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2911,7 +3174,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixing columns to add the ID primary keys we want
</commit_message>
<xml_diff>
--- a/GameDB.xlsx
+++ b/GameDB.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8EA64400-2C76-4C12-BA04-BE1C7D02B5BB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84595451-1685-46D6-A000-256473BACE71}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Game" sheetId="2" r:id="rId1"/>
@@ -16,7 +16,7 @@
     <sheet name="Manufacturer" sheetId="4" r:id="rId6"/>
     <sheet name="ESRB" sheetId="6" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -715,8 +715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA4E4693-5428-408F-9669-A33411403D4D}">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="B51" sqref="B2:B51"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2339,8 +2339,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB34F316-239A-4088-B766-2DFF3070945E}">
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2373,6 +2373,9 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
       <c r="E2" s="2">
         <v>1</v>
       </c>
@@ -2381,246 +2384,393 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
       <c r="H3" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
       <c r="H4" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
       <c r="H5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
       <c r="H6" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
       <c r="H7" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
       <c r="H8" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
       <c r="H9" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
       <c r="H10" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
       <c r="H11" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
       <c r="H12" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
       <c r="H13" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
       <c r="H14" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
       <c r="H15" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
       <c r="H16" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
       <c r="H17" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
       <c r="H18" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="19" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
       <c r="H19" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="20" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
       <c r="H20" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
       <c r="H21" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
       <c r="H22" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="23" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
       <c r="H23" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="24" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
       <c r="H24" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
       <c r="H25" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="26" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
       <c r="H26" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="27" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
       <c r="H27" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="28" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
       <c r="H28" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="29" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
       <c r="H29" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="30" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
       <c r="H30" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="31" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
       <c r="H31" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="32" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
       <c r="H32" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="33" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
       <c r="H33" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="34" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
       <c r="H34" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="35" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
       <c r="H35" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="36" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
       <c r="H36" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="37" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
       <c r="H37" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="38" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
       <c r="H38" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="39" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
       <c r="H39" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="40" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
       <c r="H40" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="41" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
       <c r="H41" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="42" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
       <c r="H42" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="43" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
       <c r="H43" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="44" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
       <c r="H44" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="45" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
       <c r="H45" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="46" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
       <c r="H46" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="47" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
       <c r="H47" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="48" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
       <c r="H48" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="49" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
       <c r="H49" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="50" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
       <c r="H50" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="51" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
       <c r="H51" t="s">
         <v>100</v>
       </c>
@@ -2634,8 +2784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68B12098-D1F7-4CF5-AB86-01DD720B5D86}">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3026,7 +3176,7 @@
   <dimension ref="B3:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:I9"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3118,18 +3268,19 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F04D5C45-7585-4A32-8023-6A6A92791153}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3137,44 +3288,64 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D2" t="str">
+        <f>"INSERT ESRB(ESRB_ID, ESRB_NAME) VALUES ('"&amp;A2&amp;"','"&amp;B2&amp;"')"</f>
+        <v>INSERT ESRB(ESRB_ID, ESRB_NAME) VALUES ('1','E')</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D6" si="0">"INSERT ESRB(ESRB_ID, ESRB_NAME) VALUES ('"&amp;A3&amp;"','"&amp;B3&amp;"')"</f>
+        <v>INSERT ESRB(ESRB_ID, ESRB_NAME) VALUES ('2','E 10+')</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT ESRB(ESRB_ID, ESRB_NAME) VALUES ('3','T')</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT ESRB(ESRB_ID, ESRB_NAME) VALUES ('4','M')</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>16</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT ESRB(ESRB_ID, ESRB_NAME) VALUES ('5','KA')</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GamesGenre xls insert statements
</commit_message>
<xml_diff>
--- a/GameDB.xlsx
+++ b/GameDB.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Game" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="118">
   <si>
     <t xml:space="preserve">GameID</t>
   </si>
@@ -199,6 +199,9 @@
     <t xml:space="preserve">GenreID</t>
   </si>
   <si>
+    <t xml:space="preserve">GenreName</t>
+  </si>
+  <si>
     <t xml:space="preserve">'Role Playing Game'</t>
   </si>
   <si>
@@ -223,9 +226,6 @@
     <t xml:space="preserve">'Music'</t>
   </si>
   <si>
-    <t xml:space="preserve">'Final Fantasy IX'</t>
-  </si>
-  <si>
     <t xml:space="preserve">'Third Person Shooter'</t>
   </si>
   <si>
@@ -241,9 +241,6 @@
     <t xml:space="preserve">'Fighting'</t>
   </si>
   <si>
-    <t xml:space="preserve">GenreName</t>
-  </si>
-  <si>
     <t xml:space="preserve">CatalogueID</t>
   </si>
   <si>
@@ -256,6 +253,12 @@
     <t xml:space="preserve">Collectable</t>
   </si>
   <si>
+    <t xml:space="preserve">NULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ManufactererID</t>
+  </si>
+  <si>
     <t xml:space="preserve">ConsoleName</t>
   </si>
   <si>
@@ -295,9 +298,6 @@
     <t xml:space="preserve">Atari 5200</t>
   </si>
   <si>
-    <t xml:space="preserve">NULL</t>
-  </si>
-  <si>
     <t xml:space="preserve">Game Cube</t>
   </si>
   <si>
@@ -332,9 +332,6 @@
   </si>
   <si>
     <t xml:space="preserve">WonderSwan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ManufactererID</t>
   </si>
   <si>
     <t xml:space="preserve">INSERT @Console (ConsoleID,ManufacturerID, ConsoleName) VALUES ('523','6','Wonder Swan')</t>
@@ -481,12 +478,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -509,7 +506,7 @@
   <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B57" activeCellId="1" sqref="A1:C51 B57"/>
+      <selection pane="topLeft" activeCell="B57" activeCellId="1" sqref="E53:E61 B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1404,10 +1401,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F52"/>
+  <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="A1:C51 D2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E53" activeCellId="0" sqref="E53:E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1420,7 +1417,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.67"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>55</v>
       </c>
@@ -1430,646 +1427,781 @@
       <c r="C1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="0" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="B2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D2" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E2" s="0" t="str">
+        <f aca="false">"INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('"&amp;A2&amp;"','"&amp;B2&amp;"','"&amp;C2&amp;"')"</f>
+        <v>INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('1','1','1')</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="B3" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="D3" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E3" s="0" t="str">
+        <f aca="false">"INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('"&amp;A3&amp;"','"&amp;B3&amp;"','"&amp;C3&amp;"')"</f>
+        <v>INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('2','1','2')</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="B4" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="D4" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E4" s="0" t="str">
+        <f aca="false">"INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('"&amp;A4&amp;"','"&amp;B4&amp;"','"&amp;C4&amp;"')"</f>
+        <v>INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('3','1','3')</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="B5" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="D5" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E5" s="0" t="str">
+        <f aca="false">"INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('"&amp;A5&amp;"','"&amp;B5&amp;"','"&amp;C5&amp;"')"</f>
+        <v>INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('4','1','4')</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
       <c r="B6" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="D6" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E6" s="0" t="str">
+        <f aca="false">"INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('"&amp;A6&amp;"','"&amp;B6&amp;"','"&amp;C6&amp;"')"</f>
+        <v>INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('5','1','5')</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
       <c r="B7" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="D7" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E7" s="0" t="str">
+        <f aca="false">"INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('"&amp;A7&amp;"','"&amp;B7&amp;"','"&amp;C7&amp;"')"</f>
+        <v>INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('6','1','6')</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
       <c r="B8" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="D8" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E8" s="0" t="str">
+        <f aca="false">"INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('"&amp;A8&amp;"','"&amp;B8&amp;"','"&amp;C8&amp;"')"</f>
+        <v>INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('7','1','7')</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
       <c r="B9" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="D9" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E9" s="0" t="str">
+        <f aca="false">"INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('"&amp;A9&amp;"','"&amp;B9&amp;"','"&amp;C9&amp;"')"</f>
+        <v>INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('8','1','8')</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
       <c r="B10" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="D10" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="E10" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="F10" s="0" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E10" s="0" t="str">
+        <f aca="false">"INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('"&amp;A10&amp;"','"&amp;B10&amp;"','"&amp;C10&amp;"')"</f>
+        <v>INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('9','1','9')</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
       <c r="B11" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="D11" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="F11" s="0" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E11" s="0" t="str">
+        <f aca="false">"INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('"&amp;A11&amp;"','"&amp;B11&amp;"','"&amp;C11&amp;"')"</f>
+        <v>INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('10','1','10')</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
       <c r="B12" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="D12" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="F12" s="0" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E12" s="0" t="str">
+        <f aca="false">"INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('"&amp;A12&amp;"','"&amp;B12&amp;"','"&amp;C12&amp;"')"</f>
+        <v>INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('11','1','11')</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
       <c r="B13" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="D13" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="F13" s="0" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E13" s="0" t="str">
+        <f aca="false">"INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('"&amp;A13&amp;"','"&amp;B13&amp;"','"&amp;C13&amp;"')"</f>
+        <v>INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('12','1','12')</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
       <c r="B14" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="D14" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="F14" s="0" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E14" s="0" t="str">
+        <f aca="false">"INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('"&amp;A14&amp;"','"&amp;B14&amp;"','"&amp;C14&amp;"')"</f>
+        <v>INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('13','1','13')</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
       <c r="B15" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="D15" s="0" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E15" s="0" t="str">
+        <f aca="false">"INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('"&amp;A15&amp;"','"&amp;B15&amp;"','"&amp;C15&amp;"')"</f>
+        <v>INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('14','1','14')</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
       <c r="B16" s="0" t="n">
         <v>9</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="D16" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E16" s="0" t="str">
+        <f aca="false">"INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('"&amp;A16&amp;"','"&amp;B16&amp;"','"&amp;C16&amp;"')"</f>
+        <v>INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('15','9','15')</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
       <c r="B17" s="0" t="n">
         <v>7</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="D17" s="0" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E17" s="0" t="str">
+        <f aca="false">"INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('"&amp;A17&amp;"','"&amp;B17&amp;"','"&amp;C17&amp;"')"</f>
+        <v>INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('16','7','16')</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
       <c r="B18" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E18" s="0" t="str">
+        <f aca="false">"INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('"&amp;A18&amp;"','"&amp;B18&amp;"','"&amp;C18&amp;"')"</f>
+        <v>INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('17','4','17')</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
       <c r="B19" s="0" t="n">
         <v>9</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>17</v>
       </c>
-      <c r="D19" s="0" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E19" s="0" t="str">
+        <f aca="false">"INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('"&amp;A19&amp;"','"&amp;B19&amp;"','"&amp;C19&amp;"')"</f>
+        <v>INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('18','9','17')</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
       <c r="B20" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="D20" s="0" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E20" s="0" t="str">
+        <f aca="false">"INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('"&amp;A20&amp;"','"&amp;B20&amp;"','"&amp;C20&amp;"')"</f>
+        <v>INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('19','4','18')</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
       <c r="B21" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>19</v>
       </c>
-      <c r="D21" s="0" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E21" s="0" t="str">
+        <f aca="false">"INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('"&amp;A21&amp;"','"&amp;B21&amp;"','"&amp;C21&amp;"')"</f>
+        <v>INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('20','4','19')</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
       <c r="B22" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C22" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="D22" s="0" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E22" s="0" t="str">
+        <f aca="false">"INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('"&amp;A22&amp;"','"&amp;B22&amp;"','"&amp;C22&amp;"')"</f>
+        <v>INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('21','4','20')</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
       <c r="B23" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C23" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="D23" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E23" s="0" t="str">
+        <f aca="false">"INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('"&amp;A23&amp;"','"&amp;B23&amp;"','"&amp;C23&amp;"')"</f>
+        <v>INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('22','4','21')</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
       <c r="B24" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C24" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="D24" s="0" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E24" s="0" t="str">
+        <f aca="false">"INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('"&amp;A24&amp;"','"&amp;B24&amp;"','"&amp;C24&amp;"')"</f>
+        <v>INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('23','4','22')</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
       <c r="B25" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C25" s="0" t="n">
         <v>23</v>
       </c>
-      <c r="D25" s="0" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E25" s="0" t="str">
+        <f aca="false">"INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('"&amp;A25&amp;"','"&amp;B25&amp;"','"&amp;C25&amp;"')"</f>
+        <v>INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('24','4','23')</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
       <c r="B26" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C26" s="0" t="n">
         <v>24</v>
       </c>
-      <c r="D26" s="0" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E26" s="0" t="str">
+        <f aca="false">"INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('"&amp;A26&amp;"','"&amp;B26&amp;"','"&amp;C26&amp;"')"</f>
+        <v>INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('25','4','24')</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
       <c r="B27" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C27" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="D27" s="0" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E27" s="0" t="str">
+        <f aca="false">"INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('"&amp;A27&amp;"','"&amp;B27&amp;"','"&amp;C27&amp;"')"</f>
+        <v>INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('26','4','25')</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
       <c r="B28" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C28" s="0" t="n">
         <v>26</v>
       </c>
-      <c r="D28" s="0" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E28" s="0" t="str">
+        <f aca="false">"INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('"&amp;A28&amp;"','"&amp;B28&amp;"','"&amp;C28&amp;"')"</f>
+        <v>INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('27','4','26')</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
       <c r="B29" s="0" t="n">
         <v>8</v>
       </c>
       <c r="C29" s="0" t="n">
         <v>27</v>
       </c>
-      <c r="D29" s="0" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E29" s="0" t="str">
+        <f aca="false">"INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('"&amp;A29&amp;"','"&amp;B29&amp;"','"&amp;C29&amp;"')"</f>
+        <v>INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('28','8','27')</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
       <c r="B30" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C30" s="0" t="n">
         <v>28</v>
       </c>
-      <c r="D30" s="0" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E30" s="0" t="str">
+        <f aca="false">"INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('"&amp;A30&amp;"','"&amp;B30&amp;"','"&amp;C30&amp;"')"</f>
+        <v>INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('29','1','28')</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
       <c r="B31" s="0" t="n">
         <v>12</v>
       </c>
       <c r="C31" s="0" t="n">
         <v>29</v>
       </c>
-      <c r="D31" s="0" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E31" s="0" t="str">
+        <f aca="false">"INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('"&amp;A31&amp;"','"&amp;B31&amp;"','"&amp;C31&amp;"')"</f>
+        <v>INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('30','12','29')</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
       <c r="B32" s="0" t="n">
         <v>12</v>
       </c>
       <c r="C32" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="D32" s="0" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E32" s="0" t="str">
+        <f aca="false">"INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('"&amp;A32&amp;"','"&amp;B32&amp;"','"&amp;C32&amp;"')"</f>
+        <v>INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('31','12','30')</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
       <c r="B33" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C33" s="0" t="n">
         <v>31</v>
       </c>
-      <c r="D33" s="0" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E33" s="0" t="str">
+        <f aca="false">"INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('"&amp;A33&amp;"','"&amp;B33&amp;"','"&amp;C33&amp;"')"</f>
+        <v>INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('32','4','31')</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
       <c r="B34" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C34" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="D34" s="0" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E34" s="0" t="str">
+        <f aca="false">"INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('"&amp;A34&amp;"','"&amp;B34&amp;"','"&amp;C34&amp;"')"</f>
+        <v>INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('33','1','32')</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
       <c r="B35" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C35" s="0" t="n">
         <v>33</v>
       </c>
-      <c r="D35" s="0" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E35" s="0" t="str">
+        <f aca="false">"INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('"&amp;A35&amp;"','"&amp;B35&amp;"','"&amp;C35&amp;"')"</f>
+        <v>INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('34','1','33')</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
       <c r="B36" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C36" s="0" t="n">
         <v>34</v>
       </c>
-      <c r="D36" s="0" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E36" s="0" t="str">
+        <f aca="false">"INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('"&amp;A36&amp;"','"&amp;B36&amp;"','"&amp;C36&amp;"')"</f>
+        <v>INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('35','1','34')</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
       <c r="B37" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C37" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="D37" s="0" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E37" s="0" t="str">
+        <f aca="false">"INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('"&amp;A37&amp;"','"&amp;B37&amp;"','"&amp;C37&amp;"')"</f>
+        <v>INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('36','1','35')</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
       <c r="B38" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C38" s="0" t="n">
         <v>36</v>
       </c>
-      <c r="D38" s="0" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E38" s="0" t="str">
+        <f aca="false">"INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('"&amp;A38&amp;"','"&amp;B38&amp;"','"&amp;C38&amp;"')"</f>
+        <v>INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('37','1','36')</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
       <c r="B39" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C39" s="0" t="n">
         <v>37</v>
       </c>
-      <c r="D39" s="0" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E39" s="0" t="str">
+        <f aca="false">"INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('"&amp;A39&amp;"','"&amp;B39&amp;"','"&amp;C39&amp;"')"</f>
+        <v>INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('38','1','37')</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
       <c r="B40" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C40" s="0" t="n">
         <v>38</v>
       </c>
-      <c r="D40" s="0" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E40" s="0" t="str">
+        <f aca="false">"INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('"&amp;A40&amp;"','"&amp;B40&amp;"','"&amp;C40&amp;"')"</f>
+        <v>INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('39','4','38')</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
       <c r="B41" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C41" s="0" t="n">
         <v>39</v>
       </c>
-      <c r="D41" s="0" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E41" s="0" t="str">
+        <f aca="false">"INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('"&amp;A41&amp;"','"&amp;B41&amp;"','"&amp;C41&amp;"')"</f>
+        <v>INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('40','4','39')</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
       <c r="B42" s="0" t="n">
         <v>7</v>
       </c>
       <c r="C42" s="0" t="n">
         <v>40</v>
       </c>
-      <c r="D42" s="0" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E42" s="0" t="str">
+        <f aca="false">"INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('"&amp;A42&amp;"','"&amp;B42&amp;"','"&amp;C42&amp;"')"</f>
+        <v>INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('41','7','40')</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
       <c r="B43" s="0" t="n">
         <v>7</v>
       </c>
       <c r="C43" s="0" t="n">
         <v>41</v>
       </c>
-      <c r="D43" s="0" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E43" s="0" t="str">
+        <f aca="false">"INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('"&amp;A43&amp;"','"&amp;B43&amp;"','"&amp;C43&amp;"')"</f>
+        <v>INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('42','7','41')</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
       <c r="B44" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C44" s="0" t="n">
         <v>42</v>
       </c>
-      <c r="D44" s="0" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E44" s="0" t="str">
+        <f aca="false">"INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('"&amp;A44&amp;"','"&amp;B44&amp;"','"&amp;C44&amp;"')"</f>
+        <v>INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('43','1','42')</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
       <c r="B45" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C45" s="0" t="n">
         <v>43</v>
       </c>
-      <c r="D45" s="0" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E45" s="0" t="str">
+        <f aca="false">"INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('"&amp;A45&amp;"','"&amp;B45&amp;"','"&amp;C45&amp;"')"</f>
+        <v>INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('44','1','43')</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
       <c r="B46" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C46" s="0" t="n">
         <v>44</v>
       </c>
-      <c r="D46" s="0" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E46" s="0" t="str">
+        <f aca="false">"INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('"&amp;A46&amp;"','"&amp;B46&amp;"','"&amp;C46&amp;"')"</f>
+        <v>INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('45','1','44')</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
       <c r="B47" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C47" s="0" t="n">
         <v>45</v>
       </c>
-      <c r="D47" s="0" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E47" s="0" t="str">
+        <f aca="false">"INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('"&amp;A47&amp;"','"&amp;B47&amp;"','"&amp;C47&amp;"')"</f>
+        <v>INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('46','1','45')</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
       <c r="B48" s="0" t="n">
         <v>7</v>
       </c>
       <c r="C48" s="0" t="n">
         <v>46</v>
       </c>
-      <c r="D48" s="0" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E48" s="0" t="str">
+        <f aca="false">"INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('"&amp;A48&amp;"','"&amp;B48&amp;"','"&amp;C48&amp;"')"</f>
+        <v>INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('47','7','46')</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
       <c r="B49" s="0" t="n">
         <v>7</v>
       </c>
       <c r="C49" s="0" t="n">
         <v>47</v>
       </c>
-      <c r="D49" s="0" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E49" s="0" t="str">
+        <f aca="false">"INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('"&amp;A49&amp;"','"&amp;B49&amp;"','"&amp;C49&amp;"')"</f>
+        <v>INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('48','7','47')</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
       <c r="B50" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C50" s="0" t="n">
         <v>48</v>
       </c>
-      <c r="D50" s="0" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E50" s="0" t="str">
+        <f aca="false">"INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('"&amp;A50&amp;"','"&amp;B50&amp;"','"&amp;C50&amp;"')"</f>
+        <v>INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('49','1','48')</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
       <c r="B51" s="0" t="n">
         <v>12</v>
       </c>
       <c r="C51" s="0" t="n">
         <v>49</v>
       </c>
-      <c r="D51" s="0" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E51" s="0" t="str">
+        <f aca="false">"INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('"&amp;A51&amp;"','"&amp;B51&amp;"','"&amp;C51&amp;"')"</f>
+        <v>INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('50','12','49')</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="n">
+        <v>51</v>
+      </c>
       <c r="B52" s="0" t="n">
         <v>3</v>
       </c>
       <c r="C52" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="D52" s="0" t="s">
-        <v>54</v>
-      </c>
-    </row>
+      <c r="E52" s="0" t="str">
+        <f aca="false">"INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('"&amp;A52&amp;"','"&amp;B52&amp;"','"&amp;C52&amp;"')"</f>
+        <v>INSERT @GameGenre (GameGenreID, GenreID, GameID) VALUES ('51','3','50')</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2089,7 +2221,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="A1:C51"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="E53:E61 B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2104,7 +2236,7 @@
         <v>56</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2112,7 +2244,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2120,7 +2252,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2128,7 +2260,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2136,7 +2268,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2144,7 +2276,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2152,7 +2284,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2160,7 +2292,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2168,7 +2300,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2227,10 +2359,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K51"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A21" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:C51"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A35" activeCellId="1" sqref="E53:E61 A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2250,31 +2382,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="0" t="s">
+      <c r="D1" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="J1" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="K1" s="0" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2289,18 +2409,6 @@
       </c>
       <c r="E2" s="1" t="n">
         <v>1</v>
-      </c>
-      <c r="G2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="J2" s="0" t="n">
-        <v>500</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2313,17 +2421,8 @@
       <c r="C3" s="0" t="n">
         <v>523</v>
       </c>
-      <c r="G3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="J3" s="0" t="n">
-        <v>501</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>78</v>
+      <c r="E3" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2336,17 +2435,8 @@
       <c r="C4" s="0" t="n">
         <v>521</v>
       </c>
-      <c r="G4" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="J4" s="0" t="n">
-        <v>502</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>79</v>
+      <c r="E4" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2359,17 +2449,8 @@
       <c r="C5" s="0" t="n">
         <v>523</v>
       </c>
-      <c r="G5" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="J5" s="0" t="n">
-        <v>503</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>80</v>
+      <c r="E5" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2382,17 +2463,8 @@
       <c r="C6" s="0" t="n">
         <v>501</v>
       </c>
-      <c r="G6" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="H6" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="J6" s="0" t="n">
-        <v>504</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>81</v>
+      <c r="E6" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2402,20 +2474,11 @@
       <c r="B7" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="C7" s="3" t="n">
+      <c r="C7" s="2" t="n">
         <v>518</v>
       </c>
-      <c r="G7" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="H7" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="J7" s="0" t="n">
-        <v>505</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>82</v>
+      <c r="E7" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2425,20 +2488,11 @@
       <c r="B8" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="C8" s="3" t="n">
+      <c r="C8" s="2" t="n">
         <v>501</v>
       </c>
-      <c r="G8" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="H8" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="J8" s="0" t="n">
-        <v>506</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>83</v>
+      <c r="E8" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2448,20 +2502,11 @@
       <c r="B9" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="C9" s="3" t="n">
+      <c r="C9" s="2" t="n">
         <v>501</v>
       </c>
-      <c r="G9" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="H9" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="J9" s="0" t="n">
-        <v>507</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>84</v>
+      <c r="E9" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2474,17 +2519,8 @@
       <c r="C10" s="0" t="n">
         <v>502</v>
       </c>
-      <c r="G10" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="H10" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="J10" s="0" t="n">
-        <v>508</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>85</v>
+      <c r="E10" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2494,20 +2530,11 @@
       <c r="B11" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="C11" s="3" t="n">
+      <c r="C11" s="2" t="n">
         <v>503</v>
       </c>
-      <c r="G11" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="H11" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="J11" s="0" t="n">
-        <v>509</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>86</v>
+      <c r="E11" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2520,17 +2547,8 @@
       <c r="C12" s="0" t="n">
         <v>507</v>
       </c>
-      <c r="G12" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="H12" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="J12" s="0" t="n">
-        <v>510</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>87</v>
+      <c r="E12" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2543,17 +2561,8 @@
       <c r="C13" s="0" t="n">
         <v>504</v>
       </c>
-      <c r="G13" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="H13" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="J13" s="0" t="n">
-        <v>511</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>88</v>
+      <c r="E13" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2564,19 +2573,10 @@
         <v>13</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="G14" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="H14" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="J14" s="0" t="n">
-        <v>512</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>90</v>
+        <v>75</v>
+      </c>
+      <c r="E14" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2589,17 +2589,8 @@
       <c r="C15" s="0" t="n">
         <v>505</v>
       </c>
-      <c r="G15" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="H15" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="J15" s="0" t="n">
-        <v>513</v>
-      </c>
-      <c r="K15" s="2" t="s">
-        <v>91</v>
+      <c r="E15" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2612,17 +2603,8 @@
       <c r="C16" s="0" t="n">
         <v>511</v>
       </c>
-      <c r="G16" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="H16" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="J16" s="0" t="n">
-        <v>514</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>92</v>
+      <c r="E16" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2635,17 +2617,8 @@
       <c r="C17" s="0" t="n">
         <v>512</v>
       </c>
-      <c r="G17" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="H17" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="J17" s="0" t="n">
-        <v>515</v>
-      </c>
-      <c r="K17" s="2" t="s">
-        <v>93</v>
+      <c r="E17" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2656,19 +2629,10 @@
         <v>17</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="G18" s="0" t="n">
-        <v>17</v>
-      </c>
-      <c r="H18" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="J18" s="0" t="n">
-        <v>516</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>94</v>
+        <v>75</v>
+      </c>
+      <c r="E18" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2679,19 +2643,10 @@
         <v>18</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="G19" s="0" t="n">
-        <v>18</v>
-      </c>
-      <c r="H19" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="J19" s="0" t="n">
-        <v>517</v>
-      </c>
-      <c r="K19" s="2" t="s">
-        <v>95</v>
+        <v>75</v>
+      </c>
+      <c r="E19" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2702,19 +2657,10 @@
         <v>19</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="G20" s="0" t="n">
-        <v>19</v>
-      </c>
-      <c r="H20" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="J20" s="0" t="n">
-        <v>518</v>
-      </c>
-      <c r="K20" s="2" t="s">
-        <v>96</v>
+        <v>75</v>
+      </c>
+      <c r="E20" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2727,17 +2673,8 @@
       <c r="C21" s="0" t="n">
         <v>507</v>
       </c>
-      <c r="G21" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="H21" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="J21" s="0" t="n">
-        <v>519</v>
-      </c>
-      <c r="K21" s="2" t="s">
-        <v>97</v>
+      <c r="E21" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2750,17 +2687,8 @@
       <c r="C22" s="0" t="n">
         <v>507</v>
       </c>
-      <c r="G22" s="0" t="n">
-        <v>21</v>
-      </c>
-      <c r="H22" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="J22" s="0" t="n">
-        <v>520</v>
-      </c>
-      <c r="K22" s="2" t="s">
-        <v>98</v>
+      <c r="E22" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2773,17 +2701,8 @@
       <c r="C23" s="0" t="n">
         <v>507</v>
       </c>
-      <c r="G23" s="0" t="n">
-        <v>22</v>
-      </c>
-      <c r="H23" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="J23" s="0" t="n">
-        <v>521</v>
-      </c>
-      <c r="K23" s="2" t="s">
-        <v>99</v>
+      <c r="E23" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2796,17 +2715,8 @@
       <c r="C24" s="0" t="n">
         <v>507</v>
       </c>
-      <c r="G24" s="0" t="n">
-        <v>23</v>
-      </c>
-      <c r="H24" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="J24" s="0" t="n">
-        <v>522</v>
-      </c>
-      <c r="K24" s="2" t="s">
-        <v>100</v>
+      <c r="E24" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2819,17 +2729,8 @@
       <c r="C25" s="0" t="n">
         <v>508</v>
       </c>
-      <c r="G25" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="H25" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="J25" s="0" t="n">
-        <v>523</v>
-      </c>
-      <c r="K25" s="2" t="s">
-        <v>101</v>
+      <c r="E25" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2842,11 +2743,8 @@
       <c r="C26" s="0" t="n">
         <v>508</v>
       </c>
-      <c r="G26" s="0" t="n">
-        <v>25</v>
-      </c>
-      <c r="H26" s="0" t="s">
-        <v>29</v>
+      <c r="E26" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2859,17 +2757,8 @@
       <c r="C27" s="0" t="n">
         <v>508</v>
       </c>
-      <c r="G27" s="0" t="n">
-        <v>26</v>
-      </c>
-      <c r="H27" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="J27" s="0" t="n">
-        <v>500</v>
-      </c>
-      <c r="K27" s="2" t="s">
-        <v>77</v>
+      <c r="E27" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2882,17 +2771,8 @@
       <c r="C28" s="0" t="n">
         <v>519</v>
       </c>
-      <c r="G28" s="0" t="n">
-        <v>27</v>
-      </c>
-      <c r="H28" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="J28" s="0" t="n">
-        <v>501</v>
-      </c>
-      <c r="K28" s="2" t="s">
-        <v>78</v>
+      <c r="E28" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2905,17 +2785,8 @@
       <c r="C29" s="0" t="n">
         <v>508</v>
       </c>
-      <c r="G29" s="0" t="n">
-        <v>28</v>
-      </c>
-      <c r="H29" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="J29" s="0" t="n">
-        <v>502</v>
-      </c>
-      <c r="K29" s="2" t="s">
-        <v>79</v>
+      <c r="E29" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2928,17 +2799,8 @@
       <c r="C30" s="0" t="n">
         <v>522</v>
       </c>
-      <c r="G30" s="0" t="n">
-        <v>29</v>
-      </c>
-      <c r="H30" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="J30" s="0" t="n">
-        <v>503</v>
-      </c>
-      <c r="K30" s="2" t="s">
-        <v>80</v>
+      <c r="E30" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2951,17 +2813,8 @@
       <c r="C31" s="0" t="n">
         <v>513</v>
       </c>
-      <c r="G31" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="H31" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="J31" s="0" t="n">
-        <v>504</v>
-      </c>
-      <c r="K31" s="2" t="s">
-        <v>81</v>
+      <c r="E31" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2974,17 +2827,8 @@
       <c r="C32" s="0" t="n">
         <v>507</v>
       </c>
-      <c r="G32" s="0" t="n">
-        <v>31</v>
-      </c>
-      <c r="H32" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="J32" s="0" t="n">
-        <v>505</v>
-      </c>
-      <c r="K32" s="2" t="s">
-        <v>82</v>
+      <c r="E32" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2995,19 +2839,10 @@
         <v>32</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="G33" s="0" t="n">
-        <v>32</v>
-      </c>
-      <c r="H33" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="J33" s="0" t="n">
-        <v>506</v>
-      </c>
-      <c r="K33" s="2" t="s">
-        <v>83</v>
+        <v>75</v>
+      </c>
+      <c r="E33" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3018,19 +2853,10 @@
         <v>33</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="G34" s="0" t="n">
-        <v>33</v>
-      </c>
-      <c r="H34" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="J34" s="0" t="n">
-        <v>507</v>
-      </c>
-      <c r="K34" s="2" t="s">
-        <v>84</v>
+        <v>75</v>
+      </c>
+      <c r="E34" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3043,17 +2869,8 @@
       <c r="C35" s="0" t="n">
         <v>506</v>
       </c>
-      <c r="G35" s="0" t="n">
-        <v>34</v>
-      </c>
-      <c r="H35" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="J35" s="0" t="n">
-        <v>508</v>
-      </c>
-      <c r="K35" s="2" t="s">
-        <v>85</v>
+      <c r="E35" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3066,17 +2883,8 @@
       <c r="C36" s="0" t="n">
         <v>507</v>
       </c>
-      <c r="G36" s="0" t="n">
-        <v>35</v>
-      </c>
-      <c r="H36" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="J36" s="0" t="n">
-        <v>509</v>
-      </c>
-      <c r="K36" s="2" t="s">
-        <v>86</v>
+      <c r="E36" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3089,17 +2897,8 @@
       <c r="C37" s="0" t="n">
         <v>508</v>
       </c>
-      <c r="G37" s="0" t="n">
-        <v>36</v>
-      </c>
-      <c r="H37" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="J37" s="0" t="n">
-        <v>510</v>
-      </c>
-      <c r="K37" s="2" t="s">
-        <v>87</v>
+      <c r="E37" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3112,17 +2911,8 @@
       <c r="C38" s="0" t="n">
         <v>508</v>
       </c>
-      <c r="G38" s="0" t="n">
-        <v>37</v>
-      </c>
-      <c r="H38" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="J38" s="0" t="n">
-        <v>511</v>
-      </c>
-      <c r="K38" s="2" t="s">
-        <v>88</v>
+      <c r="E38" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3135,17 +2925,8 @@
       <c r="C39" s="0" t="n">
         <v>505</v>
       </c>
-      <c r="G39" s="0" t="n">
-        <v>38</v>
-      </c>
-      <c r="H39" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="J39" s="0" t="n">
-        <v>512</v>
-      </c>
-      <c r="K39" s="2" t="s">
-        <v>90</v>
+      <c r="E39" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3158,17 +2939,8 @@
       <c r="C40" s="0" t="n">
         <v>505</v>
       </c>
-      <c r="G40" s="0" t="n">
-        <v>39</v>
-      </c>
-      <c r="H40" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="J40" s="0" t="n">
-        <v>513</v>
-      </c>
-      <c r="K40" s="2" t="s">
-        <v>91</v>
+      <c r="E40" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3181,17 +2953,8 @@
       <c r="C41" s="0" t="n">
         <v>513</v>
       </c>
-      <c r="G41" s="0" t="n">
-        <v>40</v>
-      </c>
-      <c r="H41" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="J41" s="0" t="n">
-        <v>514</v>
-      </c>
-      <c r="K41" s="2" t="s">
-        <v>92</v>
+      <c r="E41" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3204,17 +2967,8 @@
       <c r="C42" s="0" t="n">
         <v>500</v>
       </c>
-      <c r="G42" s="0" t="n">
-        <v>41</v>
-      </c>
-      <c r="H42" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="J42" s="0" t="n">
-        <v>515</v>
-      </c>
-      <c r="K42" s="2" t="s">
-        <v>93</v>
+      <c r="E42" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3227,17 +2981,8 @@
       <c r="C43" s="0" t="n">
         <v>521</v>
       </c>
-      <c r="G43" s="0" t="n">
-        <v>42</v>
-      </c>
-      <c r="H43" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="J43" s="0" t="n">
-        <v>516</v>
-      </c>
-      <c r="K43" s="2" t="s">
-        <v>94</v>
+      <c r="E43" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3250,17 +2995,8 @@
       <c r="C44" s="0" t="n">
         <v>522</v>
       </c>
-      <c r="G44" s="0" t="n">
-        <v>43</v>
-      </c>
-      <c r="H44" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="J44" s="0" t="n">
-        <v>517</v>
-      </c>
-      <c r="K44" s="2" t="s">
-        <v>95</v>
+      <c r="E44" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3273,17 +3009,8 @@
       <c r="C45" s="0" t="n">
         <v>522</v>
       </c>
-      <c r="G45" s="0" t="n">
-        <v>44</v>
-      </c>
-      <c r="H45" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="J45" s="0" t="n">
-        <v>518</v>
-      </c>
-      <c r="K45" s="2" t="s">
-        <v>96</v>
+      <c r="E45" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3296,17 +3023,8 @@
       <c r="C46" s="0" t="n">
         <v>516</v>
       </c>
-      <c r="G46" s="0" t="n">
-        <v>45</v>
-      </c>
-      <c r="H46" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="J46" s="0" t="n">
-        <v>519</v>
-      </c>
-      <c r="K46" s="2" t="s">
-        <v>97</v>
+      <c r="E46" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3319,17 +3037,8 @@
       <c r="C47" s="0" t="n">
         <v>522</v>
       </c>
-      <c r="G47" s="0" t="n">
-        <v>46</v>
-      </c>
-      <c r="H47" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="J47" s="0" t="n">
-        <v>520</v>
-      </c>
-      <c r="K47" s="2" t="s">
-        <v>98</v>
+      <c r="E47" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3342,17 +3051,8 @@
       <c r="C48" s="0" t="n">
         <v>522</v>
       </c>
-      <c r="G48" s="0" t="n">
-        <v>47</v>
-      </c>
-      <c r="H48" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="J48" s="0" t="n">
-        <v>521</v>
-      </c>
-      <c r="K48" s="2" t="s">
-        <v>99</v>
+      <c r="E48" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3365,17 +3065,8 @@
       <c r="C49" s="0" t="n">
         <v>504</v>
       </c>
-      <c r="G49" s="0" t="n">
-        <v>48</v>
-      </c>
-      <c r="H49" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="J49" s="0" t="n">
-        <v>522</v>
-      </c>
-      <c r="K49" s="2" t="s">
-        <v>100</v>
+      <c r="E49" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3388,17 +3079,8 @@
       <c r="C50" s="0" t="n">
         <v>506</v>
       </c>
-      <c r="G50" s="0" t="n">
-        <v>49</v>
-      </c>
-      <c r="H50" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="J50" s="0" t="n">
-        <v>523</v>
-      </c>
-      <c r="K50" s="2" t="s">
-        <v>101</v>
+      <c r="E50" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3411,11 +3093,8 @@
       <c r="C51" s="0" t="n">
         <v>509</v>
       </c>
-      <c r="G51" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="H51" s="0" t="s">
-        <v>54</v>
+      <c r="E51" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3437,7 +3116,7 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:C51"/>
+      <selection pane="topLeft" activeCell="H2" activeCellId="1" sqref="E53:E61 H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3451,24 +3130,24 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>102</v>
+        <v>76</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>500</v>
       </c>
-      <c r="B2" s="2" t="n">
+      <c r="B2" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>77</v>
+      <c r="C2" s="3" t="s">
+        <v>78</v>
       </c>
       <c r="H2" s="0" t="str">
         <f aca="false">"INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('"&amp;A2&amp;"','"&amp;B2&amp;"','"&amp;C2&amp;"')"</f>
@@ -3479,11 +3158,11 @@
       <c r="A3" s="0" t="n">
         <v>501</v>
       </c>
-      <c r="B3" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>78</v>
+      <c r="B3" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="H3" s="0" t="str">
         <f aca="false">"INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('"&amp;A3&amp;"','"&amp;B3&amp;"','"&amp;C3&amp;"')"</f>
@@ -3494,11 +3173,11 @@
       <c r="A4" s="0" t="n">
         <v>502</v>
       </c>
-      <c r="B4" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>79</v>
+      <c r="B4" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>80</v>
       </c>
       <c r="H4" s="0" t="str">
         <f aca="false">"INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('"&amp;A4&amp;"','"&amp;B4&amp;"','"&amp;C4&amp;"')"</f>
@@ -3509,11 +3188,11 @@
       <c r="A5" s="0" t="n">
         <v>503</v>
       </c>
-      <c r="B5" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>80</v>
+      <c r="B5" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>81</v>
       </c>
       <c r="H5" s="0" t="str">
         <f aca="false">"INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('"&amp;A5&amp;"','"&amp;B5&amp;"','"&amp;C5&amp;"')"</f>
@@ -3524,11 +3203,11 @@
       <c r="A6" s="0" t="n">
         <v>504</v>
       </c>
-      <c r="B6" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>81</v>
+      <c r="B6" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>82</v>
       </c>
       <c r="H6" s="0" t="str">
         <f aca="false">"INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('"&amp;A6&amp;"','"&amp;B6&amp;"','"&amp;C6&amp;"')"</f>
@@ -3539,11 +3218,11 @@
       <c r="A7" s="0" t="n">
         <v>505</v>
       </c>
-      <c r="B7" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>82</v>
+      <c r="B7" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>83</v>
       </c>
       <c r="H7" s="0" t="str">
         <f aca="false">"INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('"&amp;A7&amp;"','"&amp;B7&amp;"','"&amp;C7&amp;"')"</f>
@@ -3554,11 +3233,11 @@
       <c r="A8" s="0" t="n">
         <v>506</v>
       </c>
-      <c r="B8" s="2" t="n">
+      <c r="B8" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>83</v>
+      <c r="C8" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="H8" s="0" t="str">
         <f aca="false">"INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('"&amp;A8&amp;"','"&amp;B8&amp;"','"&amp;C8&amp;"')"</f>
@@ -3569,11 +3248,11 @@
       <c r="A9" s="0" t="n">
         <v>507</v>
       </c>
-      <c r="B9" s="2" t="n">
+      <c r="B9" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>84</v>
+      <c r="C9" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="H9" s="0" t="str">
         <f aca="false">"INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('"&amp;A9&amp;"','"&amp;B9&amp;"','"&amp;C9&amp;"')"</f>
@@ -3584,11 +3263,11 @@
       <c r="A10" s="0" t="n">
         <v>508</v>
       </c>
-      <c r="B10" s="2" t="n">
+      <c r="B10" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>85</v>
+      <c r="C10" s="3" t="s">
+        <v>86</v>
       </c>
       <c r="H10" s="0" t="str">
         <f aca="false">"INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('"&amp;A10&amp;"','"&amp;B10&amp;"','"&amp;C10&amp;"')"</f>
@@ -3599,11 +3278,11 @@
       <c r="A11" s="0" t="n">
         <v>509</v>
       </c>
-      <c r="B11" s="2" t="n">
+      <c r="B11" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>86</v>
+      <c r="C11" s="3" t="s">
+        <v>87</v>
       </c>
       <c r="H11" s="0" t="str">
         <f aca="false">"INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('"&amp;A11&amp;"','"&amp;B11&amp;"','"&amp;C11&amp;"')"</f>
@@ -3614,11 +3293,11 @@
       <c r="A12" s="0" t="n">
         <v>510</v>
       </c>
-      <c r="B12" s="2" t="n">
+      <c r="B12" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>87</v>
+      <c r="C12" s="3" t="s">
+        <v>88</v>
       </c>
       <c r="H12" s="0" t="str">
         <f aca="false">"INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('"&amp;A12&amp;"','"&amp;B12&amp;"','"&amp;C12&amp;"')"</f>
@@ -3629,11 +3308,11 @@
       <c r="A13" s="0" t="n">
         <v>511</v>
       </c>
-      <c r="B13" s="2" t="n">
+      <c r="B13" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>88</v>
+      <c r="C13" s="3" t="s">
+        <v>89</v>
       </c>
       <c r="H13" s="0" t="str">
         <f aca="false">"INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('"&amp;A13&amp;"','"&amp;B13&amp;"','"&amp;C13&amp;"')"</f>
@@ -3644,10 +3323,10 @@
       <c r="A14" s="0" t="n">
         <v>512</v>
       </c>
-      <c r="B14" s="2" t="n">
+      <c r="B14" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="3" t="s">
         <v>90</v>
       </c>
       <c r="H14" s="0" t="str">
@@ -3659,10 +3338,10 @@
       <c r="A15" s="0" t="n">
         <v>513</v>
       </c>
-      <c r="B15" s="2" t="n">
+      <c r="B15" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="3" t="s">
         <v>91</v>
       </c>
       <c r="H15" s="0" t="str">
@@ -3674,10 +3353,10 @@
       <c r="A16" s="0" t="n">
         <v>514</v>
       </c>
-      <c r="B16" s="2" t="n">
+      <c r="B16" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="3" t="s">
         <v>92</v>
       </c>
       <c r="H16" s="0" t="str">
@@ -3689,10 +3368,10 @@
       <c r="A17" s="0" t="n">
         <v>515</v>
       </c>
-      <c r="B17" s="2" t="n">
+      <c r="B17" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="3" t="s">
         <v>93</v>
       </c>
       <c r="H17" s="0" t="str">
@@ -3704,10 +3383,10 @@
       <c r="A18" s="0" t="n">
         <v>516</v>
       </c>
-      <c r="B18" s="2" t="n">
+      <c r="B18" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="3" t="s">
         <v>94</v>
       </c>
       <c r="H18" s="0" t="str">
@@ -3719,10 +3398,10 @@
       <c r="A19" s="0" t="n">
         <v>517</v>
       </c>
-      <c r="B19" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C19" s="2" t="s">
+      <c r="B19" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>95</v>
       </c>
       <c r="H19" s="0" t="str">
@@ -3734,10 +3413,10 @@
       <c r="A20" s="0" t="n">
         <v>518</v>
       </c>
-      <c r="B20" s="2" t="n">
+      <c r="B20" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="3" t="s">
         <v>96</v>
       </c>
       <c r="H20" s="0" t="str">
@@ -3749,10 +3428,10 @@
       <c r="A21" s="0" t="n">
         <v>519</v>
       </c>
-      <c r="B21" s="2" t="n">
+      <c r="B21" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="3" t="s">
         <v>97</v>
       </c>
       <c r="H21" s="0" t="str">
@@ -3764,10 +3443,10 @@
       <c r="A22" s="0" t="n">
         <v>520</v>
       </c>
-      <c r="B22" s="2" t="n">
+      <c r="B22" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="3" t="s">
         <v>98</v>
       </c>
       <c r="H22" s="0" t="str">
@@ -3779,10 +3458,10 @@
       <c r="A23" s="0" t="n">
         <v>521</v>
       </c>
-      <c r="B23" s="2" t="n">
+      <c r="B23" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="3" t="s">
         <v>99</v>
       </c>
       <c r="H23" s="0" t="str">
@@ -3794,10 +3473,10 @@
       <c r="A24" s="0" t="n">
         <v>522</v>
       </c>
-      <c r="B24" s="2" t="n">
+      <c r="B24" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="3" t="s">
         <v>100</v>
       </c>
       <c r="H24" s="0" t="str">
@@ -3809,14 +3488,14 @@
       <c r="A25" s="0" t="n">
         <v>523</v>
       </c>
-      <c r="B25" s="2" t="n">
+      <c r="B25" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="3" t="s">
         <v>101</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -3838,7 +3517,7 @@
   <dimension ref="B3:I9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I4" activeCellId="1" sqref="A1:C51 I4"/>
+      <selection pane="topLeft" activeCell="I4" activeCellId="1" sqref="E53:E61 I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3848,18 +3527,18 @@
   <sheetData>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>104</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>106</v>
+      <c r="C4" s="3" t="s">
+        <v>105</v>
       </c>
       <c r="I4" s="0" t="str">
         <f aca="false">"INSERT @Manufacturer (ManufacturerID, ManufacturerName) VALUES ('"&amp;B4&amp;"','"&amp;C4&amp;"')"</f>
@@ -3870,8 +3549,8 @@
       <c r="B5" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>107</v>
+      <c r="C5" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="I5" s="0" t="str">
         <f aca="false">"INSERT @Manufacturer (ManufacturerID, ManufacturerName) VALUES ('"&amp;B5&amp;"','"&amp;C5&amp;"')"</f>
@@ -3882,8 +3561,8 @@
       <c r="B6" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>108</v>
+      <c r="C6" s="3" t="s">
+        <v>107</v>
       </c>
       <c r="I6" s="0" t="str">
         <f aca="false">"INSERT @Manufacturer (ManufacturerID, ManufacturerName) VALUES ('"&amp;B6&amp;"','"&amp;C6&amp;"')"</f>
@@ -3894,8 +3573,8 @@
       <c r="B7" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>109</v>
+      <c r="C7" s="3" t="s">
+        <v>108</v>
       </c>
       <c r="I7" s="0" t="str">
         <f aca="false">"INSERT @Manufacturer (ManufacturerID, ManufacturerName) VALUES ('"&amp;B7&amp;"','"&amp;C7&amp;"')"</f>
@@ -3906,8 +3585,8 @@
       <c r="B8" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>110</v>
+      <c r="C8" s="3" t="s">
+        <v>109</v>
       </c>
       <c r="I8" s="0" t="str">
         <f aca="false">"INSERT @Manufacturer (ManufacturerID, ManufacturerName) VALUES ('"&amp;B8&amp;"','"&amp;C8&amp;"')"</f>
@@ -3918,8 +3597,8 @@
       <c r="B9" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>111</v>
+      <c r="C9" s="3" t="s">
+        <v>110</v>
       </c>
       <c r="I9" s="0" t="str">
         <f aca="false">"INSERT @Manufacturer (ManufacturerID, ManufacturerName) VALUES ('"&amp;B9&amp;"','"&amp;C9&amp;"')"</f>
@@ -3945,7 +3624,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="A1:C51"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="1" sqref="E53:E61 C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3958,10 +3637,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" s="0" t="s">
         <v>112</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3969,7 +3648,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D2" s="0" t="str">
         <f aca="false">"INSERT ESRB(ESRB_ID, ESRB_NAME) VALUES ('"&amp;A2&amp;"','"&amp;B2&amp;"')"</f>
@@ -3981,7 +3660,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D3" s="0" t="str">
         <f aca="false">"INSERT ESRB(ESRB_ID, ESRB_NAME) VALUES ('"&amp;A3&amp;"','"&amp;B3&amp;"')"</f>
@@ -3993,7 +3672,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D4" s="0" t="str">
         <f aca="false">"INSERT ESRB(ESRB_ID, ESRB_NAME) VALUES ('"&amp;A4&amp;"','"&amp;B4&amp;"')"</f>
@@ -4005,7 +3684,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D5" s="0" t="str">
         <f aca="false">"INSERT ESRB(ESRB_ID, ESRB_NAME) VALUES ('"&amp;A5&amp;"','"&amp;B5&amp;"')"</f>
@@ -4017,7 +3696,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D6" s="0" t="str">
         <f aca="false">"INSERT ESRB(ESRB_ID, ESRB_NAME) VALUES ('"&amp;A6&amp;"','"&amp;B6&amp;"')"</f>

</xml_diff>

<commit_message>
drop tables from outside in
</commit_message>
<xml_diff>
--- a/GameDB.xlsx
+++ b/GameDB.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Game" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="119">
   <si>
     <t xml:space="preserve">GameID</t>
   </si>
@@ -67,7 +67,7 @@
     <t xml:space="preserve">'Final Fantasy VIII'</t>
   </si>
   <si>
-    <t xml:space="preserve">'Final FantasyIX'</t>
+    <t xml:space="preserve">'Final Fantasy IX'</t>
   </si>
   <si>
     <t xml:space="preserve">'Final Fantasy X'</t>
@@ -142,7 +142,7 @@
     <t xml:space="preserve">'Elder Scrolls II: Daggerfall'</t>
   </si>
   <si>
-    <t xml:space="preserve">'Elder Scrolls III: Marrowind'</t>
+    <t xml:space="preserve">'Elder Scrolls III: Morrowind'</t>
   </si>
   <si>
     <t xml:space="preserve">'Elder Scrolls IV: Oblivion'</t>
@@ -251,6 +251,9 @@
   </si>
   <si>
     <t xml:space="preserve">Collectable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note NULL Console ID defaults to PC</t>
   </si>
   <si>
     <t xml:space="preserve">NULL</t>
@@ -505,14 +508,14 @@
   </sheetPr>
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B57" activeCellId="0" sqref="B57"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.67"/>
@@ -719,7 +722,7 @@
         <v>0</v>
       </c>
       <c r="E12" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1403,7 +1406,7 @@
   </sheetPr>
   <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E53" activeCellId="0" sqref="E53"/>
     </sheetView>
   </sheetViews>
@@ -2220,7 +2223,7 @@
   </sheetPr>
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -2359,10 +2362,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2410,6 +2413,9 @@
       <c r="E2" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="H2" s="0" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
@@ -2573,7 +2579,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E14" s="1" t="n">
         <v>0</v>
@@ -2629,7 +2635,7 @@
         <v>17</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E18" s="1" t="n">
         <v>0</v>
@@ -2643,7 +2649,7 @@
         <v>18</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E19" s="1" t="n">
         <v>0</v>
@@ -2657,7 +2663,7 @@
         <v>19</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E20" s="1" t="n">
         <v>0</v>
@@ -2839,7 +2845,7 @@
         <v>32</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E33" s="1" t="n">
         <v>0</v>
@@ -2853,7 +2859,7 @@
         <v>33</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E34" s="1" t="n">
         <v>0</v>
@@ -3113,33 +3119,34 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1021" min="5" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1022" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>72</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>500</v>
       </c>
@@ -3147,14 +3154,14 @@
         <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="H2" s="0" t="str">
+        <v>79</v>
+      </c>
+      <c r="E2" s="0" t="str">
         <f aca="false">"INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('"&amp;A2&amp;"','"&amp;B2&amp;"','"&amp;C2&amp;"')"</f>
         <v>INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('500','4','Sega Genesis')</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>501</v>
       </c>
@@ -3162,14 +3169,14 @@
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="H3" s="0" t="str">
+        <v>80</v>
+      </c>
+      <c r="E3" s="0" t="str">
         <f aca="false">"INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('"&amp;A3&amp;"','"&amp;B3&amp;"','"&amp;C3&amp;"')"</f>
         <v>INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('501','1','PlayStation ')</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>502</v>
       </c>
@@ -3177,14 +3184,14 @@
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="H4" s="0" t="str">
+        <v>81</v>
+      </c>
+      <c r="E4" s="0" t="str">
         <f aca="false">"INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('"&amp;A4&amp;"','"&amp;B4&amp;"','"&amp;C4&amp;"')"</f>
         <v>INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('502','1','PlayStation 1')</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>503</v>
       </c>
@@ -3192,14 +3199,14 @@
         <v>1</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="H5" s="0" t="str">
+        <v>82</v>
+      </c>
+      <c r="E5" s="0" t="str">
         <f aca="false">"INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('"&amp;A5&amp;"','"&amp;B5&amp;"','"&amp;C5&amp;"')"</f>
         <v>INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('503','1','PlayStation 2')</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>504</v>
       </c>
@@ -3207,14 +3214,14 @@
         <v>1</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="H6" s="0" t="str">
+        <v>83</v>
+      </c>
+      <c r="E6" s="0" t="str">
         <f aca="false">"INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('"&amp;A6&amp;"','"&amp;B6&amp;"','"&amp;C6&amp;"')"</f>
         <v>INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('504','1','PlayStation 3')</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>505</v>
       </c>
@@ -3222,14 +3229,14 @@
         <v>1</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="H7" s="0" t="str">
+        <v>84</v>
+      </c>
+      <c r="E7" s="0" t="str">
         <f aca="false">"INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('"&amp;A7&amp;"','"&amp;B7&amp;"','"&amp;C7&amp;"')"</f>
         <v>INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('505','1','PlayStation 4')</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>506</v>
       </c>
@@ -3237,14 +3244,14 @@
         <v>3</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="H8" s="0" t="str">
+        <v>85</v>
+      </c>
+      <c r="E8" s="0" t="str">
         <f aca="false">"INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('"&amp;A8&amp;"','"&amp;B8&amp;"','"&amp;C8&amp;"')"</f>
         <v>INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('506','3','Xbox')</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>507</v>
       </c>
@@ -3252,14 +3259,14 @@
         <v>3</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="H9" s="0" t="str">
+        <v>86</v>
+      </c>
+      <c r="E9" s="0" t="str">
         <f aca="false">"INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('"&amp;A9&amp;"','"&amp;B9&amp;"','"&amp;C9&amp;"')"</f>
         <v>INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('507','3','Xbox 360')</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>508</v>
       </c>
@@ -3267,14 +3274,14 @@
         <v>3</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="H10" s="0" t="str">
+        <v>87</v>
+      </c>
+      <c r="E10" s="0" t="str">
         <f aca="false">"INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('"&amp;A10&amp;"','"&amp;B10&amp;"','"&amp;C10&amp;"')"</f>
         <v>INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('508','3','Xbox One')</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <v>509</v>
       </c>
@@ -3282,14 +3289,14 @@
         <v>5</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="H11" s="0" t="str">
+        <v>88</v>
+      </c>
+      <c r="E11" s="0" t="str">
         <f aca="false">"INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('"&amp;A11&amp;"','"&amp;B11&amp;"','"&amp;C11&amp;"')"</f>
         <v>INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('509','5','Atari 2600')</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>510</v>
       </c>
@@ -3297,14 +3304,14 @@
         <v>5</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="H12" s="0" t="str">
+        <v>89</v>
+      </c>
+      <c r="E12" s="0" t="str">
         <f aca="false">"INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('"&amp;A12&amp;"','"&amp;B12&amp;"','"&amp;C12&amp;"')"</f>
         <v>INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('510','5','Atari Lynx')</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>511</v>
       </c>
@@ -3312,14 +3319,14 @@
         <v>5</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="H13" s="0" t="str">
+        <v>90</v>
+      </c>
+      <c r="E13" s="0" t="str">
         <f aca="false">"INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('"&amp;A13&amp;"','"&amp;B13&amp;"','"&amp;C13&amp;"')"</f>
         <v>INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('511','5','Atari 5200')</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <v>512</v>
       </c>
@@ -3327,14 +3334,14 @@
         <v>2</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="H14" s="0" t="str">
+        <v>91</v>
+      </c>
+      <c r="E14" s="0" t="str">
         <f aca="false">"INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('"&amp;A14&amp;"','"&amp;B14&amp;"','"&amp;C14&amp;"')"</f>
         <v>INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('512','2','Game Cube')</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <v>513</v>
       </c>
@@ -3342,14 +3349,14 @@
         <v>2</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="H15" s="0" t="str">
+        <v>92</v>
+      </c>
+      <c r="E15" s="0" t="str">
         <f aca="false">"INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('"&amp;A15&amp;"','"&amp;B15&amp;"','"&amp;C15&amp;"')"</f>
         <v>INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('513','2','Wii')</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
         <v>514</v>
       </c>
@@ -3357,14 +3364,14 @@
         <v>2</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="H16" s="0" t="str">
+        <v>93</v>
+      </c>
+      <c r="E16" s="0" t="str">
         <f aca="false">"INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('"&amp;A16&amp;"','"&amp;B16&amp;"','"&amp;C16&amp;"')"</f>
         <v>INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('514','2','Wii U')</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <v>515</v>
       </c>
@@ -3372,14 +3379,14 @@
         <v>2</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="H17" s="0" t="str">
+        <v>94</v>
+      </c>
+      <c r="E17" s="0" t="str">
         <f aca="false">"INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('"&amp;A17&amp;"','"&amp;B17&amp;"','"&amp;C17&amp;"')"</f>
         <v>INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('515','2','Game Boy')</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
         <v>516</v>
       </c>
@@ -3387,14 +3394,14 @@
         <v>2</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="H18" s="0" t="str">
+        <v>95</v>
+      </c>
+      <c r="E18" s="0" t="str">
         <f aca="false">"INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('"&amp;A18&amp;"','"&amp;B18&amp;"','"&amp;C18&amp;"')"</f>
         <v>INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('516','2','Game Boy Color')</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
         <v>517</v>
       </c>
@@ -3402,14 +3409,14 @@
         <v>1</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="H19" s="0" t="str">
+        <v>96</v>
+      </c>
+      <c r="E19" s="0" t="str">
         <f aca="false">"INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('"&amp;A19&amp;"','"&amp;B19&amp;"','"&amp;C19&amp;"')"</f>
         <v>INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('517','1','PlayStation Vita')</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
         <v>518</v>
       </c>
@@ -3417,14 +3424,14 @@
         <v>2</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="H20" s="0" t="str">
+        <v>97</v>
+      </c>
+      <c r="E20" s="0" t="str">
         <f aca="false">"INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('"&amp;A20&amp;"','"&amp;B20&amp;"','"&amp;C20&amp;"')"</f>
         <v>INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('518','2','Super Nintendo')</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
         <v>519</v>
       </c>
@@ -3432,14 +3439,14 @@
         <v>2</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="H21" s="0" t="str">
+        <v>98</v>
+      </c>
+      <c r="E21" s="0" t="str">
         <f aca="false">"INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('"&amp;A21&amp;"','"&amp;B21&amp;"','"&amp;C21&amp;"')"</f>
         <v>INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('519','2','Nintendo DS')</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
         <v>520</v>
       </c>
@@ -3447,14 +3454,14 @@
         <v>2</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="H22" s="0" t="str">
+        <v>99</v>
+      </c>
+      <c r="E22" s="0" t="str">
         <f aca="false">"INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('"&amp;A22&amp;"','"&amp;B22&amp;"','"&amp;C22&amp;"')"</f>
         <v>INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('520','2','Nintendo 3DS')</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
         <v>521</v>
       </c>
@@ -3462,14 +3469,14 @@
         <v>2</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="H23" s="0" t="str">
+        <v>100</v>
+      </c>
+      <c r="E23" s="0" t="str">
         <f aca="false">"INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('"&amp;A23&amp;"','"&amp;B23&amp;"','"&amp;C23&amp;"')"</f>
         <v>INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('521','2','Nintendo Entertainment System')</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
         <v>522</v>
       </c>
@@ -3477,14 +3484,14 @@
         <v>2</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="H24" s="0" t="str">
+        <v>101</v>
+      </c>
+      <c r="E24" s="0" t="str">
         <f aca="false">"INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('"&amp;A24&amp;"','"&amp;B24&amp;"','"&amp;C24&amp;"')"</f>
         <v>INSERT @Console (ConsoleID, ManufacturerID, ConsoleName) VALUES ('522','2','Nintendo 64')</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
         <v>523</v>
       </c>
@@ -3492,10 +3499,10 @@
         <v>6</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="H25" s="0" t="s">
         <v>102</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -3514,93 +3521,94 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B3:I9"/>
+  <dimension ref="B3:E9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1020" min="1" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1021" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="I4" s="0" t="str">
+        <v>106</v>
+      </c>
+      <c r="E4" s="0" t="str">
         <f aca="false">"INSERT @Manufacturer (ManufacturerID, ManufacturerName) VALUES ('"&amp;B4&amp;"','"&amp;C4&amp;"')"</f>
         <v>INSERT @Manufacturer (ManufacturerID, ManufacturerName) VALUES ('1','Sony')</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="I5" s="0" t="str">
+        <v>107</v>
+      </c>
+      <c r="E5" s="0" t="str">
         <f aca="false">"INSERT @Manufacturer (ManufacturerID, ManufacturerName) VALUES ('"&amp;B5&amp;"','"&amp;C5&amp;"')"</f>
         <v>INSERT @Manufacturer (ManufacturerID, ManufacturerName) VALUES ('2','Nintendo')</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="n">
         <v>3</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="I6" s="0" t="str">
+        <v>108</v>
+      </c>
+      <c r="E6" s="0" t="str">
         <f aca="false">"INSERT @Manufacturer (ManufacturerID, ManufacturerName) VALUES ('"&amp;B6&amp;"','"&amp;C6&amp;"')"</f>
         <v>INSERT @Manufacturer (ManufacturerID, ManufacturerName) VALUES ('3','Microsoft')</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="I7" s="0" t="str">
+        <v>109</v>
+      </c>
+      <c r="E7" s="0" t="str">
         <f aca="false">"INSERT @Manufacturer (ManufacturerID, ManufacturerName) VALUES ('"&amp;B7&amp;"','"&amp;C7&amp;"')"</f>
         <v>INSERT @Manufacturer (ManufacturerID, ManufacturerName) VALUES ('4','Sega')</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="n">
         <v>5</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="I8" s="0" t="str">
+        <v>110</v>
+      </c>
+      <c r="E8" s="0" t="str">
         <f aca="false">"INSERT @Manufacturer (ManufacturerID, ManufacturerName) VALUES ('"&amp;B8&amp;"','"&amp;C8&amp;"')"</f>
         <v>INSERT @Manufacturer (ManufacturerID, ManufacturerName) VALUES ('5','Atari')</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="n">
         <v>6</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="I9" s="0" t="str">
+        <v>111</v>
+      </c>
+      <c r="E9" s="0" t="str">
         <f aca="false">"INSERT @Manufacturer (ManufacturerID, ManufacturerName) VALUES ('"&amp;B9&amp;"','"&amp;C9&amp;"')"</f>
         <v>INSERT @Manufacturer (ManufacturerID, ManufacturerName) VALUES ('6','Bandai')</v>
       </c>
@@ -3623,7 +3631,7 @@
   </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -3637,10 +3645,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3648,7 +3656,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D2" s="0" t="str">
         <f aca="false">"INSERT ESRB(ESRB_ID, ESRB_NAME) VALUES ('"&amp;A2&amp;"','"&amp;B2&amp;"')"</f>
@@ -3660,7 +3668,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D3" s="0" t="str">
         <f aca="false">"INSERT ESRB(ESRB_ID, ESRB_NAME) VALUES ('"&amp;A3&amp;"','"&amp;B3&amp;"')"</f>
@@ -3672,7 +3680,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D4" s="0" t="str">
         <f aca="false">"INSERT ESRB(ESRB_ID, ESRB_NAME) VALUES ('"&amp;A4&amp;"','"&amp;B4&amp;"')"</f>
@@ -3684,7 +3692,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D5" s="0" t="str">
         <f aca="false">"INSERT ESRB(ESRB_ID, ESRB_NAME) VALUES ('"&amp;A5&amp;"','"&amp;B5&amp;"')"</f>
@@ -3696,7 +3704,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D6" s="0" t="str">
         <f aca="false">"INSERT ESRB(ESRB_ID, ESRB_NAME) VALUES ('"&amp;A6&amp;"','"&amp;B6&amp;"')"</f>

</xml_diff>